<commit_message>
- Add Layers order in the PCB
</commit_message>
<xml_diff>
--- a/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
+++ b/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2B06CEF-C3DE-4209-9074-BEBFEAB3A185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C683F2A-A797-45FC-9904-344EF35450E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47985" yWindow="1860" windowWidth="21540" windowHeight="11205" xr2:uid="{AFA75C7F-10CF-4329-A474-976F12078C9D}"/>
+    <workbookView xWindow="47985" yWindow="1860" windowWidth="21540" windowHeight="11205" xr2:uid="{E1C317A7-9CFB-401E-A237-45D7FF1F8649}"/>
   </bookViews>
   <sheets>
     <sheet name="X2E Reference Sensor_Default_Bi" sheetId="1" r:id="rId1"/>
@@ -1380,7 +1380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EA0C47-F297-4410-BF7D-316463C4CE36}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C3C128-5E38-4279-AA00-90B2E683A611}">
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
- Fix the LoRa Antenna swapping - Reroute the SPI and CTRL after Swapping LoRa modules: IO48->SX1280_Busy, IO47->SX1280_SS, IO33->SX1280_DIO1, IO40->SX1280_nRES IO46->SX1261_Busy, IO41->SX1261_SS, IO45->SX1261_DIO1, IO42->SX1261_nRES - R25 10K Not fitted - Change the F1 fuse with lower resistance - Add Voltage divider resistor R26 1K because the maximum voltage at VCTL is 3V - Move Charging Status LEDs closer to each other - Move The accelerometer near to the Center and fix the axis orientation - Change the part number of the Charging socket J5
</commit_message>
<xml_diff>
--- a/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
+++ b/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C683F2A-A797-45FC-9904-344EF35450E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E389ADD9-B96D-4FC1-A870-1792A3BD61FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47985" yWindow="1860" windowWidth="21540" windowHeight="11205" xr2:uid="{E1C317A7-9CFB-401E-A237-45D7FF1F8649}"/>
+    <workbookView xWindow="46095" yWindow="15" windowWidth="28770" windowHeight="15450" xr2:uid="{F5CC3A66-7B2C-4B2E-8955-475FE08A28A8}"/>
   </bookViews>
   <sheets>
     <sheet name="X2E Reference Sensor_Default_Bi" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="324">
   <si>
     <t>Fitted</t>
   </si>
@@ -341,16 +341,19 @@
     <t>F1</t>
   </si>
   <si>
-    <t>Fuse Chip Slow Blow Acting 1A 63V SMD Solder Pad 1206 3.2 X 0.51 X 0.63mm Ceramic Automotive</t>
+    <t>108mR</t>
+  </si>
+  <si>
+    <t>Fuse Chip Slow Blow Acting 1A 63V SMD Solder Pad 1206 T/R UL</t>
   </si>
   <si>
     <t>F1206</t>
   </si>
   <si>
-    <t>Bel</t>
-  </si>
-  <si>
-    <t>C1T 1</t>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>SF-1206S100-2</t>
   </si>
   <si>
     <t>IC1</t>
@@ -521,7 +524,7 @@
     <t>JST S2B-PH-SM4-TB</t>
   </si>
   <si>
-    <t>1775469-2</t>
+    <t>S2B-PH-SM4-TB(LF)(SN)</t>
   </si>
   <si>
     <t>L1, L2, L5, L6, L15, L17</t>
@@ -716,7 +719,7 @@
     <t>AC0603FR-101KL</t>
   </si>
   <si>
-    <t>R2, R9, R22, R25, R35, R36, R42, R48, R70, R79</t>
+    <t>R2, R9, R22, R35, R36, R42, R48, R70, R79</t>
   </si>
   <si>
     <t>10k</t>
@@ -815,6 +818,12 @@
     <t>AC0603FR-135K1L</t>
   </si>
   <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>RES, 1k, 1%, 1/16 W, 0402</t>
+  </si>
+  <si>
     <t>R33, R34, R37, R38, R43, R44, R72, R73, R74, R76, R77, R78</t>
   </si>
   <si>
@@ -900,9 +909,6 @@
   </si>
   <si>
     <t>Espressif Systems</t>
-  </si>
-  <si>
-    <t>ESP32-S3-MINI-1-N8</t>
   </si>
   <si>
     <t>U2</t>
@@ -1380,8 +1386,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C3C128-5E38-4279-AA00-90B2E683A611}">
-  <dimension ref="A1:I70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8FA329-1BB9-4C81-91DD-E22E9FA2C5F3}">
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1909,952 +1915,950 @@
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="E22" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C35" s="1">
         <v>6</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="G36" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C45" s="1">
         <v>2</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>82</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>82</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C47" s="1">
         <v>1</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
       <c r="B48" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C48" s="1">
         <v>3</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C49" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C50" s="1">
         <v>4</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C52" s="1">
         <v>13</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C53" s="1">
         <v>5</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C54" s="1">
         <v>4</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C56" s="1">
         <v>4</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C57" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>259</v>
+        <v>222</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>260</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="2" t="s">
-        <v>261</v>
-      </c>
+      <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C58" s="1">
+        <v>12</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C58" s="1">
-        <v>1</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="F58" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C59" s="1">
-        <v>1</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="F59" s="2" t="s">
-        <v>269</v>
+        <v>229</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I59" s="1"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I60" s="1"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C61" s="1">
-        <v>2</v>
-      </c>
-      <c r="D61" s="1"/>
       <c r="E61" s="2" t="s">
         <v>276</v>
       </c>
       <c r="F61" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>279</v>
       </c>
       <c r="I61" s="1"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
       <c r="B62" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C62" s="1">
         <v>2</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="D62" s="1"/>
       <c r="E62" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="I62" s="1"/>
     </row>
@@ -2864,9 +2868,11 @@
         <v>283</v>
       </c>
       <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E63" s="2" t="s">
         <v>284</v>
       </c>
@@ -2874,181 +2880,204 @@
         <v>285</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>286</v>
+        <v>19</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>287</v>
+        <v>19</v>
       </c>
       <c r="I63" s="1"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
       <c r="B64" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
-      <c r="D64" s="2" t="s">
+      <c r="G64" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="H64" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I64" s="1"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1"/>
-      <c r="E65" s="2" t="s">
+      <c r="F65" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="H65" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H66" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="I67" s="1"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
       <c r="B68" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="G68" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="2" t="s">
+      <c r="H68" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
       <c r="B69" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C69" s="1">
-        <v>1</v>
-      </c>
-      <c r="D69" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="I69" s="1"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="G70" s="2" t="s">
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="I70" s="1"/>
+      <c r="F71" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="I71" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Regenerated ordering data. Changed all footprints to use metric holes.
</commit_message>
<xml_diff>
--- a/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
+++ b/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\Altium\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{656758B3-1B44-4E52-8E02-5A4B7109FD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{461F17CB-B150-4542-8C9F-75D335875145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26325" yWindow="0" windowWidth="21600" windowHeight="11505"/>
   </bookViews>
@@ -765,7 +765,7 @@
     <t>AC0603FR-101KL</t>
   </si>
   <si>
-    <t>R2, R9, R22, R35, R36, R42, R48, R70, R79</t>
+    <t>R2, R9, R35, R36, R42, R48, R70, R79</t>
   </si>
   <si>
     <t>10k</t>
@@ -2673,7 +2673,7 @@
         <v>245</v>
       </c>
       <c r="C54" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>246</v>

</xml_diff>

<commit_message>
- Fix C32 & C33 Part numbers - Add part number to R26 - Fix the flipped Designators between R8 and R21 on the PCB top overlay
</commit_message>
<xml_diff>
--- a/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
+++ b/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\Altium\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2E1CE76-2B87-4301-AE29-F68B6AD1FB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972E3D84-6D82-4BC0-B71D-AEDC6F94F695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26325" yWindow="0" windowWidth="21600" windowHeight="11505"/>
+    <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{1C4AC6C5-B86A-4D07-B83C-24C63E60FC46}"/>
   </bookViews>
   <sheets>
     <sheet name="X2E Reference Sensor_Default_Bi" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,28 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'X2E Reference Sensor_Default_Bi'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="335">
   <si>
     <t>Fitted</t>
   </si>
@@ -141,7 +152,7 @@
     <t>CAP, CERM, 12pF, 16V, +/- 5%, C0G/NP0, 0402</t>
   </si>
   <si>
-    <t>GRM0225C1C120GA03L</t>
+    <t>C0402C120K4GACTU</t>
   </si>
   <si>
     <t>C40, C79</t>
@@ -177,9 +188,6 @@
     <t>CAP, CERM, 47nF, 16V, +/- 10%, X7R, 0402</t>
   </si>
   <si>
-    <t>GCM155R71C473KA37D</t>
-  </si>
-  <si>
     <t>C84</t>
   </si>
   <si>
@@ -255,9 +263,6 @@
     <t>ON Semiconductor</t>
   </si>
   <si>
-    <t>ESD9L5.0ST5G</t>
-  </si>
-  <si>
     <t>D4</t>
   </si>
   <si>
@@ -1018,23 +1023,65 @@
   </si>
   <si>
     <t>ECS-520-12-37B-CTN-TR</t>
+  </si>
+  <si>
+    <t>From DigiKey</t>
+  </si>
+  <si>
+    <t>AC0402FR-131KL</t>
+  </si>
+  <si>
+    <t>GCM155R71C473KA37J</t>
+  </si>
+  <si>
+    <t>SESD9L5.0ST5G</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/johanson-technology-inc/0868LP15A0020001E/4824451?s=N4IgTCBcDaIAwA4BsCAyAFAjAVgIJzDgFEQBdAXyA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/jst-sales-america-inc/S2B-PH-SM4-TB/926655?s=N4IgTCBcDaIMpgEIFoAKAJZcCyAWZAKogBQAyAYgJTFwBylIAugL5A</t>
+  </si>
+  <si>
+    <t>Not Available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1047,8 +1094,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1071,18 +1128,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1394,25 +1474,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39282A79-8A7A-498D-ADC2-73B4B3EC3216}">
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="54.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.86328125" customWidth="1"/>
+    <col min="2" max="2" width="51.3984375" customWidth="1"/>
+    <col min="3" max="3" width="8.06640625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="54.3984375" customWidth="1"/>
+    <col min="6" max="6" width="25.3984375" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="9" max="9" width="15.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1441,7 +1523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -1459,12 +1541,12 @@
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -1482,12 +1564,12 @@
       <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
@@ -1505,14 +1587,14 @@
         <v>22</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="7" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>25</v>
@@ -1530,14 +1612,14 @@
         <v>22</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>29</v>
@@ -1555,14 +1637,14 @@
         <v>32</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="7" t="s">
         <v>33</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>34</v>
@@ -1580,14 +1662,14 @@
         <v>22</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="7" t="s">
         <v>37</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>38</v>
@@ -1605,14 +1687,14 @@
         <v>22</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>42</v>
@@ -1630,12 +1712,12 @@
         <v>22</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="7" t="s">
         <v>45</v>
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>46</v>
@@ -1653,665 +1735,677 @@
         <v>22</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="2" t="s">
-        <v>49</v>
+      <c r="H10" s="9" t="s">
+        <v>330</v>
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="2" t="s">
-        <v>53</v>
+      <c r="H11" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="2" t="s">
-        <v>57</v>
+      <c r="H12" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="2" t="s">
-        <v>61</v>
+      <c r="H13" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>75</v>
+      <c r="H16" s="9" t="s">
+        <v>331</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="H17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>83</v>
+      <c r="H18" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="H19" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="H20" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="H21" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="H26" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="H27" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="H28" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="H29" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="H30" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="H31" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="H32" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="H34" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="H35" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="H36" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="H37" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -2320,677 +2414,679 @@
         <v>24</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="H39" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>186</v>
+      <c r="H40" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>189</v>
+      <c r="H41" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C42" s="1">
         <v>6</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="H42" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C43" s="1">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="F43" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>196</v>
+      <c r="H43" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="H44" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="G45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C46" s="1">
         <v>2</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H46" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="G47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H47" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
       <c r="B48" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E48" s="2" t="s">
+      <c r="H48" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="H49" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C50" s="1">
         <v>2</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H50" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H51" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H52" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C53" s="1">
         <v>3</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="G53" s="1"/>
+      <c r="H53" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C54" s="1">
         <v>8</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="G54" s="1"/>
+      <c r="H54" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C55" s="1">
         <v>4</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G55" s="1"/>
+      <c r="H55" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="2" t="s">
+      <c r="F56" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G56" s="1"/>
+      <c r="H56" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C57" s="1">
         <v>13</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G57" s="1"/>
+      <c r="H57" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C58" s="1">
         <v>5</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="H58" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="2" t="s">
-        <v>265</v>
-      </c>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C59" s="1">
         <v>4</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="F60" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C61" s="1">
         <v>4</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
       <c r="B62" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
+      <c r="H62" s="8" t="s">
+        <v>329</v>
+      </c>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
       <c r="B63" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C63" s="1">
         <v>12</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
       <c r="B64" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
-      <c r="D64" s="2" t="s">
+      <c r="F64" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-      <c r="D65" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="G65" s="1"/>
+      <c r="H65" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C66" s="1">
-        <v>1</v>
-      </c>
-      <c r="D66" s="2" t="s">
+      <c r="F66" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G66" s="1"/>
+      <c r="H66" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="2" t="s">
-        <v>296</v>
-      </c>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C67" s="1">
         <v>2</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="H67" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G67" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
       <c r="B68" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C68" s="1">
         <v>2</v>
@@ -2999,10 +3095,10 @@
         <v>24</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>24</v>
@@ -3012,131 +3108,140 @@
       </c>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
       <c r="B69" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C69" s="1">
         <v>1</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>307</v>
+      <c r="H69" s="5" t="s">
+        <v>305</v>
       </c>
       <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C70" s="1">
-        <v>1</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="F70" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="H70" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="1"/>
       <c r="B71" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C71" s="1">
-        <v>1</v>
-      </c>
-      <c r="D71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="H71" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="1"/>
       <c r="B72" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="C72" s="1">
-        <v>1</v>
-      </c>
-      <c r="D72" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="H72" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="G72" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="1"/>
       <c r="B73" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="2" t="s">
+      <c r="F73" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="H73" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="I73" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H10" r:id="rId1" display="https://eu.mouser.com/ProductDetail/Murata-Electronics/GCM155R71C473KA37J?qs=N3Kl9KD794QyuG7xlAebbw%3D%3D" xr:uid="{22ED9E80-DC85-4932-8CA4-8C6CB7B4E96F}"/>
+    <hyperlink ref="H16" r:id="rId2" display="https://eu.mouser.com/ProductDetail/onsemi/SESD9L5.0ST5G?qs=Nxq7uuo%252ByTnL7r1LmzloLA%3D%3D" xr:uid="{F2CF6BD3-5F0C-4D21-B27D-993162063B39}"/>
+    <hyperlink ref="I23" r:id="rId3" xr:uid="{8BE1ABD1-D16B-4A0A-A8B2-ECC02729246C}"/>
+    <hyperlink ref="I38" r:id="rId4" xr:uid="{D491C32A-E5AC-4FF4-9057-FE2BE0FFC2BC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed some errors after running DRC
</commit_message>
<xml_diff>
--- a/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
+++ b/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\Altium\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2E1CE76-2B87-4301-AE29-F68B6AD1FB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{819DBBA9-F254-4B8F-B975-2EB8074AEA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26325" yWindow="0" windowWidth="21600" windowHeight="11505"/>
+    <workbookView xWindow="1885" yWindow="1885" windowWidth="21378" windowHeight="11387"/>
   </bookViews>
   <sheets>
     <sheet name="X2E Reference Sensor_Default_Bi" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="334">
   <si>
     <t>Fitted</t>
   </si>
@@ -87,7 +87,7 @@
     <t>PRO-OB-440</t>
   </si>
   <si>
-    <t>C1, C3, C6, C7, C10, C11, C23, C24, C25, C26, C29, C36, C38, C39, C44, C82, C83, C95, C96</t>
+    <t>C1, C3, C6, C10, C11, C23, C24, C25, C26, C29, C36, C38, C39, C44, C82, C83, C95, C96</t>
   </si>
   <si>
     <t>100 nF</t>
@@ -132,6 +132,9 @@
     <t>GRM21BR61C106KE15L</t>
   </si>
   <si>
+    <t>C7</t>
+  </si>
+  <si>
     <t>C32, C33</t>
   </si>
   <si>
@@ -228,7 +231,7 @@
     <t>C0402C102K4RAC</t>
   </si>
   <si>
-    <t>D1, D5</t>
+    <t>D1</t>
   </si>
   <si>
     <t>Red 625nm LED Indication - Discrete 2V 0603 (1608 Metric)</t>
@@ -273,456 +276,462 @@
     <t>US1GWF-7</t>
   </si>
   <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>LED Low-Power Uni-Color Red 639nm 2V 2-Pin Chip LED T/R</t>
+  </si>
+  <si>
+    <t>LED0603_RA</t>
+  </si>
+  <si>
+    <t>Vishay Lite-On</t>
+  </si>
+  <si>
+    <t>LTST-S270KRKT</t>
+  </si>
+  <si>
     <t>D6, D13</t>
   </si>
   <si>
-    <t>Green 520nm LED Indication - Discrete 3.2V 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>150060GS75000</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>Diode Schottky 40V 250mA (DC) Surface Mount SOD-523</t>
-  </si>
-  <si>
-    <t>SOD-523</t>
+    <t>LED GREEN CLEAR 0603 R/A SMD / LED Uni-Color Green 574nm 2-Pin Chip LED T/R</t>
+  </si>
+  <si>
+    <t>LTST-S270KGKT</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>TVS DIODE 15 V 0402</t>
+  </si>
+  <si>
+    <t>T0402</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>LXES1UTAA1-157</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>108mR</t>
+  </si>
+  <si>
+    <t>Fuse Chip Slow Blow Acting 1A 63V SMD Solder Pad 1206 T/R UL</t>
+  </si>
+  <si>
+    <t>F1206</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>SF-1206S100-2</t>
+  </si>
+  <si>
+    <t>FL1</t>
+  </si>
+  <si>
+    <t>Impedance-matched Filter For Sem</t>
+  </si>
+  <si>
+    <t>FP-0900FM15D0039E-MFG</t>
+  </si>
+  <si>
+    <t>Johanson</t>
+  </si>
+  <si>
+    <t>0900FM15D0039E</t>
+  </si>
+  <si>
+    <t>FL2</t>
+  </si>
+  <si>
+    <t>RF Filter - Lowpass</t>
+  </si>
+  <si>
+    <t>LP_FILTER_JOHANSON</t>
+  </si>
+  <si>
+    <t>0868LP15A020E</t>
+  </si>
+  <si>
+    <t>FL3</t>
+  </si>
+  <si>
+    <t>Rf Filter 2.4GHZ-2.5GHZ 0402</t>
+  </si>
+  <si>
+    <t>JT=2450FM07D0034T</t>
+  </si>
+  <si>
+    <t>2450FM07D0034T</t>
+  </si>
+  <si>
+    <t>FL4</t>
+  </si>
+  <si>
+    <t>Rf Filter Low Pass 2.4GHZ 0402</t>
+  </si>
+  <si>
+    <t>JT=2450LP07C0100T</t>
+  </si>
+  <si>
+    <t>2450LP07C0100T</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>IC CONTROLLR LI-ION 4.2V SOT23-5</t>
+  </si>
+  <si>
+    <t>SOT23-5</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ATI/OT</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>DC to DC Converter Buck-Boost 2.6V 1.6A 12-Pin WLP T/R</t>
+  </si>
+  <si>
+    <t>14-FC2QFN</t>
+  </si>
+  <si>
+    <t>Maxim</t>
+  </si>
+  <si>
+    <t>MAX77827DEFD+T</t>
+  </si>
+  <si>
+    <t>IC3</t>
+  </si>
+  <si>
+    <t>Accelerometer X, Y, Z Axis ±2g, 4g, 8g, 16g 0.5Hz ~ 2.69kHz 12-LGA (2x2)</t>
+  </si>
+  <si>
+    <t>LGA12C50P4X4_200X200X100</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>LIS2DE12TR</t>
+  </si>
+  <si>
+    <t>IC4</t>
+  </si>
+  <si>
+    <t>SENSOR PRESSURE HUMIDITY TEMP</t>
+  </si>
+  <si>
+    <t>LGA65P250X250-8</t>
+  </si>
+  <si>
+    <t>Bosch</t>
+  </si>
+  <si>
+    <t>BME280</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>Indoor Air Quality Sensor</t>
+  </si>
+  <si>
+    <t>ZMOD4xxx_AI1_Standard</t>
+  </si>
+  <si>
+    <t>Renesas</t>
+  </si>
+  <si>
+    <t>ZMOD4410_AI1</t>
+  </si>
+  <si>
+    <t>IC6</t>
+  </si>
+  <si>
+    <t>IC RF TxRx Only General ISM &lt; 1GHz LoRaWAN 150MHz ~ 960MHz 24-VFQFN Exposed Pad</t>
+  </si>
+  <si>
+    <t>QFN50P400X400X80_HS-25N_Semtech</t>
+  </si>
+  <si>
+    <t>Semtech</t>
+  </si>
+  <si>
+    <t>SX1261IMLTRT</t>
+  </si>
+  <si>
+    <t>IC7</t>
+  </si>
+  <si>
+    <t>RF Switch IC WLAN 6GHz 50 Ohm 6-QFN (1x1)</t>
+  </si>
+  <si>
+    <t>QFN50P100X100X50-6N</t>
+  </si>
+  <si>
+    <t>Skyworks Solutions</t>
+  </si>
+  <si>
+    <t>SKY13453-385LF</t>
+  </si>
+  <si>
+    <t>IC8</t>
+  </si>
+  <si>
+    <t>IC RF TxRx Only 802.15.4 LoRa™ 2.4GHz 24-WFQFN Exposed Pad</t>
+  </si>
+  <si>
+    <t>SX1280IMLTRT</t>
+  </si>
+  <si>
+    <t>IC9</t>
+  </si>
+  <si>
+    <t>Single cell pack/system-side CEDV battery fuel (gas) gauge w/pre-programmed chemistry profiles 9-DSBGA -40 to 85</t>
+  </si>
+  <si>
+    <t>IC_BQ27421YZFR-G1A</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>BQ27220YZFR</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>Conn USB 2.0 Type C RCP 24 POS 0.3mm/0.5mm Solder RA SMD 24 Terminal 1 Port T/R</t>
+  </si>
+  <si>
+    <t>TYPE-CF-16P-RAT-L7.3</t>
+  </si>
+  <si>
+    <t>Global Connector Technology</t>
+  </si>
+  <si>
+    <t>USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>4 Positions Header Connector 0.079" (2.00mm) Through Hole Tin</t>
+  </si>
+  <si>
+    <t>CON-NS-TECH_1125S-4P</t>
+  </si>
+  <si>
+    <t>Seeed Studio</t>
+  </si>
+  <si>
+    <t>110990030</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD R/A 4POS 2MM</t>
+  </si>
+  <si>
+    <t>JST S4B-PH-SM4-TB</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>1734827-4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 2POS 2MM</t>
+  </si>
+  <si>
+    <t>CON_S2B-PH-K-S</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>S2B-PH-K-S(LF)(SN)</t>
+  </si>
+  <si>
+    <t>J6, J9</t>
+  </si>
+  <si>
+    <t>Arduino Template</t>
+  </si>
+  <si>
+    <t>Arduino-C, Arduino-A</t>
+  </si>
+  <si>
+    <t>Harwin</t>
+  </si>
+  <si>
+    <t>M20-7820842</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Arduino-B</t>
+  </si>
+  <si>
+    <t>M20-7820646</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>Arduino-D</t>
+  </si>
+  <si>
+    <t>M20-7821042</t>
+  </si>
+  <si>
+    <t>L1, L2, L5, L6, L15, L17</t>
+  </si>
+  <si>
+    <t>Ferrite Beads 0603 600ohms 1.3A DCR=.15ohms</t>
+  </si>
+  <si>
+    <t>L0603</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>BLM18KG601SH1D</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>DLP11SA350HL2L</t>
+  </si>
+  <si>
+    <t>Common Mode Filters / Chokes 35Ohm 20% 100MHz</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>1uH/4.1A</t>
+  </si>
+  <si>
+    <t>FIXED IND 1UH 4.1A 42 MOHM SMD</t>
+  </si>
+  <si>
+    <t>L252020</t>
+  </si>
+  <si>
+    <t>Pulse</t>
+  </si>
+  <si>
+    <t>BDHE002520121R0MQ1</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>27nH</t>
+  </si>
+  <si>
+    <t>Inductor, Wirewound, 27 nH, 280mA , 520mOhm, SMD</t>
+  </si>
+  <si>
+    <t>L0402</t>
+  </si>
+  <si>
+    <t>LQW15AN27NJ00D</t>
+  </si>
+  <si>
+    <t>L12, L14</t>
+  </si>
+  <si>
+    <t>47nH</t>
+  </si>
+  <si>
+    <t>Inductor, Wirewound, 47nH, 210 mA, 1.08Ohms, ±0.2nH, SMD</t>
+  </si>
+  <si>
+    <t>LQW15AN47NJ00D</t>
+  </si>
+  <si>
+    <t>L13</t>
+  </si>
+  <si>
+    <t>15uH</t>
+  </si>
+  <si>
+    <t>Inductor, 15Uh, 0.25A, Multilayer Rohs Compliant: Yes</t>
+  </si>
+  <si>
+    <t>L0805_ML</t>
+  </si>
+  <si>
+    <t>LQM21DN150M70L</t>
+  </si>
+  <si>
+    <t>L16</t>
+  </si>
+  <si>
+    <t>Chip inductor, 15uH, 250mA, 950mOhm, 0805</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>MLZ2012M150WTD25</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>CONN UMCC JACK STR 50OHM SMD</t>
+  </si>
+  <si>
+    <t>CON_U.FL</t>
+  </si>
+  <si>
+    <t>TE Connectivity AMP Connectors</t>
+  </si>
+  <si>
+    <t>1909763-1</t>
+  </si>
+  <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t>MOSFETN-CH 30V 6.2A SOT23-3</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
   </si>
   <si>
     <t>Diodes</t>
   </si>
   <si>
-    <t>SDM20U40-7</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>TVS DIODE 15 V 0402</t>
-  </si>
-  <si>
-    <t>T0402</t>
-  </si>
-  <si>
-    <t>Murata</t>
-  </si>
-  <si>
-    <t>LXES1UTAA1-157</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>108mR</t>
-  </si>
-  <si>
-    <t>Fuse Chip Slow Blow Acting 1A 63V SMD Solder Pad 1206 T/R UL</t>
-  </si>
-  <si>
-    <t>F1206</t>
-  </si>
-  <si>
-    <t>Bourns</t>
-  </si>
-  <si>
-    <t>SF-1206S100-2</t>
-  </si>
-  <si>
-    <t>FL1</t>
-  </si>
-  <si>
-    <t>Impedance-matched Filter For Sem</t>
-  </si>
-  <si>
-    <t>FP-0900FM15D0039E-MFG</t>
-  </si>
-  <si>
-    <t>Johanson</t>
-  </si>
-  <si>
-    <t>0900FM15D0039E</t>
-  </si>
-  <si>
-    <t>FL2</t>
-  </si>
-  <si>
-    <t>RF Filter - Lowpass</t>
-  </si>
-  <si>
-    <t>LP_FILTER_JOHANSON</t>
-  </si>
-  <si>
-    <t>0868LP15A020E</t>
-  </si>
-  <si>
-    <t>FL3</t>
-  </si>
-  <si>
-    <t>Rf Filter 2.4GHZ-2.5GHZ 0402</t>
-  </si>
-  <si>
-    <t>JT=2450FM07D0034T</t>
-  </si>
-  <si>
-    <t>2450FM07D0034T</t>
-  </si>
-  <si>
-    <t>FL4</t>
-  </si>
-  <si>
-    <t>Rf Filter Low Pass 2.4GHZ 0402</t>
-  </si>
-  <si>
-    <t>JT=2450LP07C0100T</t>
-  </si>
-  <si>
-    <t>2450LP07C0100T</t>
-  </si>
-  <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>IC CONTROLLR LI-ION 4.2V SOT23-5</t>
-  </si>
-  <si>
-    <t>SOT23-5</t>
-  </si>
-  <si>
-    <t>Microchip</t>
-  </si>
-  <si>
-    <t>MCP73831T-2ATI/OT</t>
-  </si>
-  <si>
-    <t>IC2</t>
-  </si>
-  <si>
-    <t>DC to DC Converter Buck-Boost 2.6V 1.6A 12-Pin WLP T/R</t>
-  </si>
-  <si>
-    <t>14-FC2QFN</t>
-  </si>
-  <si>
-    <t>Maxim</t>
-  </si>
-  <si>
-    <t>MAX77827DEFD+T</t>
-  </si>
-  <si>
-    <t>IC3</t>
-  </si>
-  <si>
-    <t>Accelerometer X, Y, Z Axis ±2g, 4g, 8g, 16g 0.5Hz ~ 2.69kHz 12-LGA (2x2)</t>
-  </si>
-  <si>
-    <t>LGA12C50P4X4_200X200X100</t>
-  </si>
-  <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
-    <t>LIS2DE12TR</t>
-  </si>
-  <si>
-    <t>IC4</t>
-  </si>
-  <si>
-    <t>SENSOR PRESSURE HUMIDITY TEMP</t>
-  </si>
-  <si>
-    <t>LGA65P250X250-8</t>
-  </si>
-  <si>
-    <t>Bosch</t>
-  </si>
-  <si>
-    <t>BME280</t>
-  </si>
-  <si>
-    <t>IC5</t>
-  </si>
-  <si>
-    <t>Indoor Air Quality Sensor</t>
-  </si>
-  <si>
-    <t>ZMOD4xxx_AI1_Standard</t>
-  </si>
-  <si>
-    <t>Renesas</t>
-  </si>
-  <si>
-    <t>ZMOD4410_AI1</t>
-  </si>
-  <si>
-    <t>IC6</t>
-  </si>
-  <si>
-    <t>IC RF TxRx Only General ISM &lt; 1GHz LoRaWAN 150MHz ~ 960MHz 24-VFQFN Exposed Pad</t>
-  </si>
-  <si>
-    <t>QFN50P400X400X80_HS-25N_Semtech</t>
-  </si>
-  <si>
-    <t>Semtech</t>
-  </si>
-  <si>
-    <t>SX1261IMLTRT</t>
-  </si>
-  <si>
-    <t>IC7</t>
-  </si>
-  <si>
-    <t>RF Switch IC WLAN 6GHz 50 Ohm 6-QFN (1x1)</t>
-  </si>
-  <si>
-    <t>QFN50P100X100X50-6N</t>
-  </si>
-  <si>
-    <t>Skyworks Solutions</t>
-  </si>
-  <si>
-    <t>SKY13453-385LF</t>
-  </si>
-  <si>
-    <t>IC8</t>
-  </si>
-  <si>
-    <t>IC RF TxRx Only 802.15.4 LoRa™ 2.4GHz 24-WFQFN Exposed Pad</t>
-  </si>
-  <si>
-    <t>SX1280IMLTRT</t>
-  </si>
-  <si>
-    <t>IC9</t>
-  </si>
-  <si>
-    <t>Single cell pack/system-side CEDV battery fuel (gas) gauge w/pre-programmed chemistry profiles 9-DSBGA -40 to 85</t>
-  </si>
-  <si>
-    <t>IC_BQ27421YZFR-G1A</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>BQ27220YZFR</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>Conn USB 2.0 Type C RCP 24 POS 0.3mm/0.5mm Solder RA SMD 24 Terminal 1 Port T/R</t>
-  </si>
-  <si>
-    <t>TYPE-CF-16P-RAT-L7.3</t>
-  </si>
-  <si>
-    <t>Global Connector Technology</t>
-  </si>
-  <si>
-    <t>USB4105-GF-A</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>4 Positions Header Connector 0.079" (2.00mm) Through Hole Tin</t>
-  </si>
-  <si>
-    <t>CON-NS-TECH_1125S-4P</t>
-  </si>
-  <si>
-    <t>Seeed Studio</t>
-  </si>
-  <si>
-    <t>110990030</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>CONN HEADER SMD R/A 4POS 2MM</t>
-  </si>
-  <si>
-    <t>JST S4B-PH-SM4-TB</t>
-  </si>
-  <si>
-    <t>JST Sales America Inc.</t>
-  </si>
-  <si>
-    <t>1734827-4</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>CONN HEADER SMD R/A 2POS 2MM</t>
-  </si>
-  <si>
-    <t>JST S2B-PH-SM4-TB</t>
-  </si>
-  <si>
-    <t>S2B-PH-SM4-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>J6, J9</t>
-  </si>
-  <si>
-    <t>Arduino Template</t>
-  </si>
-  <si>
-    <t>Arduino-C, Arduino-A</t>
-  </si>
-  <si>
-    <t>Harwin</t>
-  </si>
-  <si>
-    <t>M20-7820842</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Arduino-B</t>
-  </si>
-  <si>
-    <t>M20-7820646</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>Arduino-D</t>
-  </si>
-  <si>
-    <t>M20-7821042</t>
-  </si>
-  <si>
-    <t>L1, L2, L5, L6, L15, L17</t>
-  </si>
-  <si>
-    <t>Ferrite Beads 0603 600ohms 1.3A DCR=.15ohms</t>
-  </si>
-  <si>
-    <t>L0603</t>
-  </si>
-  <si>
-    <t>Murata Electronics North America</t>
-  </si>
-  <si>
-    <t>BLM18KG601SH1D</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>DLP11SA350HL2L</t>
-  </si>
-  <si>
-    <t>Common Mode Filters / Chokes 35Ohm 20% 100MHz</t>
-  </si>
-  <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>1uH/4.1A</t>
-  </si>
-  <si>
-    <t>FIXED IND 1UH 4.1A 42 MOHM SMD</t>
-  </si>
-  <si>
-    <t>L252020</t>
-  </si>
-  <si>
-    <t>Pulse</t>
-  </si>
-  <si>
-    <t>BDHE002520121R0MQ1</t>
-  </si>
-  <si>
-    <t>L7</t>
-  </si>
-  <si>
-    <t>27nH</t>
-  </si>
-  <si>
-    <t>Inductor, Wirewound, 27 nH, 280mA , 520mOhm, SMD</t>
-  </si>
-  <si>
-    <t>L0402</t>
-  </si>
-  <si>
-    <t>LQW15AN27NJ00D</t>
-  </si>
-  <si>
-    <t>L12, L14</t>
-  </si>
-  <si>
-    <t>47nH</t>
-  </si>
-  <si>
-    <t>Inductor, Wirewound, 47nH, 210 mA, 1.08Ohms, ±0.2nH, SMD</t>
-  </si>
-  <si>
-    <t>LQW15AN47NJ00D</t>
-  </si>
-  <si>
-    <t>L13</t>
-  </si>
-  <si>
-    <t>15uH</t>
-  </si>
-  <si>
-    <t>Inductor, 15Uh, 0.25A, Multilayer Rohs Compliant: Yes</t>
-  </si>
-  <si>
-    <t>L0805_ML</t>
-  </si>
-  <si>
-    <t>LQM21DN150M70L</t>
-  </si>
-  <si>
-    <t>L16</t>
-  </si>
-  <si>
-    <t>Chip inductor, 15uH, 250mA, 950mOhm, 0805</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>MLZ2012M150WTD25</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>CONN UMCC JACK STR 50OHM SMD</t>
-  </si>
-  <si>
-    <t>CON_U.FL</t>
-  </si>
-  <si>
-    <t>TE Connectivity AMP Connectors</t>
-  </si>
-  <si>
-    <t>1909763-1</t>
-  </si>
-  <si>
-    <t>Q1, Q2</t>
-  </si>
-  <si>
-    <t>MOSFETN-CH 30V 6.2A SOT23-3</t>
-  </si>
-  <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
     <t>DMN3023L-7</t>
   </si>
   <si>
@@ -862,6 +871,9 @@
   </si>
   <si>
     <t>AC0603FR-135K1L</t>
+  </si>
+  <si>
+    <t>R22</t>
   </si>
   <si>
     <t>R26</t>
@@ -1395,21 +1407,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="54.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1493,7 +1505,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>20</v>
@@ -1568,45 +1580,41 @@
         <v>34</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>24</v>
@@ -1615,117 +1623,117 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>24</v>
@@ -1734,693 +1742,693 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C39" s="1">
-        <v>2</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C42" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43" s="1">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>196</v>
@@ -2430,710 +2438,756 @@
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="F44" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="H44" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C46" s="1">
-        <v>2</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="G46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="F47" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E48" s="2" t="s">
+      <c r="G48" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C49" s="1">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C51" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="G52" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C53" s="1">
-        <v>3</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="F53" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C54" s="1">
-        <v>8</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C55" s="1">
+        <v>8</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C55" s="1">
-        <v>4</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="F56" s="2" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C57" s="1">
-        <v>13</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="F57" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C58" s="1">
+        <v>13</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C58" s="1">
-        <v>5</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="F58" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C59" s="1">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C59" s="1">
-        <v>4</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="F59" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I59" s="1"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C60" s="1">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C60" s="1">
-        <v>1</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>272</v>
-      </c>
       <c r="F60" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I60" s="1"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C61" s="1">
-        <v>4</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="F61" s="2" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I61" s="1"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C62" s="1">
+        <v>4</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>279</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
+      <c r="H62" s="2" t="s">
+        <v>280</v>
+      </c>
       <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C63" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G63" s="1"/>
-      <c r="H63" s="2" t="s">
-        <v>283</v>
-      </c>
+      <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>285</v>
+        <v>244</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G64" s="1"/>
-      <c r="H64" s="2" t="s">
-        <v>287</v>
-      </c>
+      <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C65" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>291</v>
+        <v>251</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C67" s="1">
-        <v>2</v>
-      </c>
-      <c r="D67" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>293</v>
+      </c>
       <c r="E67" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>300</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="G67" s="1"/>
       <c r="H67" s="2" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I67" s="1"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C68" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>24</v>
+        <v>298</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="G68" s="1"/>
       <c r="H68" s="2" t="s">
-        <v>24</v>
+        <v>300</v>
       </c>
       <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C69" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I69" s="1"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C70" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>310</v>
+        <v>24</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>312</v>
+        <v>24</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>310</v>
+        <v>24</v>
       </c>
       <c r="I70" s="1"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C71" s="1">
         <v>1</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>314</v>
-      </c>
+      <c r="D71" s="1"/>
       <c r="E71" s="2" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="I71" s="1"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="G73" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="I73" s="1"/>
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="I75" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GPS.SchDoc - connected pin 7 of the module to V3P3_GPS through 0R, regenerated the production files.
</commit_message>
<xml_diff>
--- a/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
+++ b/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\Altium\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8A21356-9F50-4794-AA44-818CEA829794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B19C6071-7C4C-4E81-8B57-43CA55A07E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1885" yWindow="1885" windowWidth="21378" windowHeight="11387"/>
   </bookViews>
@@ -813,7 +813,7 @@
     <t>AF0603FR-073KL</t>
   </si>
   <si>
-    <t>R8, R12, R15, R21, R30, R31, R40, R49, R50, R69, R75, R83, R84</t>
+    <t>R8, R12, R15, R21, R30, R31, R39, R40, R49, R50, R69, R75, R83, R84</t>
   </si>
   <si>
     <t>0R</t>
@@ -2775,7 +2775,7 @@
         <v>261</v>
       </c>
       <c r="C58" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>262</v>

</xml_diff>

<commit_message>
Update BOM GPS module to GT-1110-UB7X.
</commit_message>
<xml_diff>
--- a/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
+++ b/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
@@ -1,34 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\Altium\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B19C6071-7C4C-4E81-8B57-43CA55A07E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="1885" yWindow="1885" windowWidth="21378" windowHeight="11387"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="X2E Reference Sensor_Default_Bi" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="X2E Reference Sensor_Default_Bi" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'X2E Reference Sensor_Default_Bi'!$1:$1</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="IJnaINjPVsrb1djT3vTMMrTqyo2diKFonkOpulFnYn0="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="335">
   <si>
     <t>Fitted</t>
   </si>
@@ -972,13 +960,16 @@
     <t>U2</t>
   </si>
   <si>
+    <t>GT-1110-UB7X</t>
+  </si>
+  <si>
+    <t>GPS Module 10.1x9.7x2.5mm 9600 Baud Rate</t>
+  </si>
+  <si>
     <t>SIM28ML</t>
   </si>
   <si>
-    <t>GPS Module 10.1x9.7x2.5mm 9600 Baud Rate</t>
-  </si>
-  <si>
-    <t>SIMCom</t>
+    <t>GOTOP</t>
   </si>
   <si>
     <t>Y1</t>
@@ -1035,15 +1026,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1051,80 +1045,79 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFD3D3D3"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
+    <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf quotePrefix="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4472C4"/>
@@ -1148,113 +1141,19 @@
         <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="0563C1"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1395,1802 +1294,2742 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="55" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="58.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="24.57"/>
+    <col customWidth="1" min="2" max="2" width="55.0"/>
+    <col customWidth="1" min="3" max="3" width="8.71"/>
+    <col customWidth="1" min="4" max="4" width="17.14"/>
+    <col customWidth="1" min="5" max="5" width="58.14"/>
+    <col customWidth="1" min="6" max="6" width="27.29"/>
+    <col customWidth="1" min="7" max="7" width="17.0"/>
+    <col customWidth="1" min="8" max="8" width="27.86"/>
+    <col customWidth="1" min="9" max="9" width="16.71"/>
+    <col customWidth="1" min="10" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="1">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="3">
+        <v>16.0</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="3"/>
+      <c r="H8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2" t="s">
+      <c r="G13" s="3"/>
+      <c r="H13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2" t="s">
+      <c r="G15" s="3"/>
+      <c r="H15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2" t="s">
+      <c r="C16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2" t="s">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="1">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2" t="s">
+      <c r="C17" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2" t="s">
+      <c r="C18" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2" t="s">
+      <c r="C19" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2" t="s">
+      <c r="C20" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2" t="s">
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2" t="s">
+      <c r="C21" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2" t="s">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="2" t="s">
+      <c r="C23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="2" t="s">
+      <c r="C24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2" t="s">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="2" t="s">
+      <c r="C25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2" t="s">
+      <c r="C26" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2" t="s">
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="2" t="s">
+      <c r="C27" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2" t="s">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="2" t="s">
+      <c r="C28" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2" t="s">
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="2" t="s">
+      <c r="C29" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2" t="s">
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="2" t="s">
+      <c r="C30" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2" t="s">
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" ht="14.25" customHeight="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="2" t="s">
+      <c r="C31" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2" t="s">
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" ht="14.25" customHeight="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="2" t="s">
+      <c r="C32" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2" t="s">
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="2" t="s">
+      <c r="C33" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2" t="s">
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="2" t="s">
+      <c r="C34" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2" t="s">
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="3"/>
+      <c r="B35" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="2" t="s">
+      <c r="C35" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2" t="s">
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="2" t="s">
+      <c r="C36" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2" t="s">
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="A37" s="3"/>
+      <c r="B37" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2" t="s">
+      <c r="C37" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2" t="s">
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="2" t="s">
+      <c r="C38" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2" t="s">
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C39" s="1">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="2" t="s">
+      <c r="C39" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2" t="s">
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" ht="14.25" customHeight="1">
+      <c r="A40" s="3"/>
+      <c r="B40" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C40" s="1">
-        <v>2</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C40" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2" t="s">
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" ht="14.25" customHeight="1">
+      <c r="A41" s="3"/>
+      <c r="B41" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="2" t="s">
+      <c r="C41" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2" t="s">
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" ht="14.25" customHeight="1">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C42" s="1">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="2" t="s">
+      <c r="C42" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2" t="s">
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" ht="14.25" customHeight="1">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="C43" s="1">
-        <v>6</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="2" t="s">
+      <c r="C43" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2" t="s">
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="C44" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="2" t="s">
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" ht="14.25" customHeight="1">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="C45" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="2" t="s">
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" ht="14.25" customHeight="1">
+      <c r="A46" s="3"/>
+      <c r="B46" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="C46" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2" t="s">
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" ht="14.25" customHeight="1">
+      <c r="A47" s="3"/>
+      <c r="B47" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C47" s="1">
-        <v>2</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="C47" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2" t="s">
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="3"/>
+      <c r="B48" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C48" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2" t="s">
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="3"/>
+      <c r="B49" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C49" s="1">
-        <v>1</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C49" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="2" t="s">
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="3"/>
+      <c r="B50" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="2" t="s">
+      <c r="C50" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2" t="s">
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" ht="14.25" customHeight="1">
+      <c r="A51" s="3"/>
+      <c r="B51" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C51" s="1">
-        <v>2</v>
-      </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="2" t="s">
+      <c r="C51" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="2" t="s">
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" ht="14.25" customHeight="1">
+      <c r="A52" s="3"/>
+      <c r="B52" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="2" t="s">
+      <c r="C52" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H52" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2" t="s">
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" ht="14.25" customHeight="1">
+      <c r="A53" s="3"/>
+      <c r="B53" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="2" t="s">
+      <c r="C53" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2" t="s">
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" ht="14.25" customHeight="1">
+      <c r="A54" s="3"/>
+      <c r="B54" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C54" s="1">
-        <v>3</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="C54" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="2" t="s">
+      <c r="G54" s="3"/>
+      <c r="H54" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="2" t="s">
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" ht="14.25" customHeight="1">
+      <c r="A55" s="3"/>
+      <c r="B55" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C55" s="1">
-        <v>8</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="C55" s="3">
+        <v>8.0</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="2" t="s">
+      <c r="G55" s="3"/>
+      <c r="H55" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2" t="s">
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" ht="14.25" customHeight="1">
+      <c r="A56" s="3"/>
+      <c r="B56" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C56" s="1">
-        <v>4</v>
-      </c>
-      <c r="D56" s="2" t="s">
+      <c r="C56" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="2" t="s">
+      <c r="G56" s="3"/>
+      <c r="H56" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="I56" s="1"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2" t="s">
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" ht="14.25" customHeight="1">
+      <c r="A57" s="3"/>
+      <c r="B57" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="C57" s="1">
-        <v>1</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="C57" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="2" t="s">
+      <c r="G57" s="3"/>
+      <c r="H57" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="2" t="s">
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" ht="14.25" customHeight="1">
+      <c r="A58" s="3"/>
+      <c r="B58" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="C58" s="1">
-        <v>14</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="C58" s="3">
+        <v>14.0</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="2" t="s">
+      <c r="G58" s="3"/>
+      <c r="H58" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="I58" s="1"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="2" t="s">
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" ht="14.25" customHeight="1">
+      <c r="A59" s="3"/>
+      <c r="B59" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="C59" s="1">
-        <v>5</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="C59" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="2" t="s">
+      <c r="G59" s="3"/>
+      <c r="H59" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="2" t="s">
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" ht="14.25" customHeight="1">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="C60" s="1">
-        <v>4</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="C60" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="2" t="s">
+      <c r="G60" s="3"/>
+      <c r="H60" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2" t="s">
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" ht="14.25" customHeight="1">
+      <c r="A61" s="3"/>
+      <c r="B61" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="C61" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F61" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="2" t="s">
+      <c r="G61" s="3"/>
+      <c r="H61" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2" t="s">
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" ht="14.25" customHeight="1">
+      <c r="A62" s="3"/>
+      <c r="B62" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="C62" s="1">
-        <v>4</v>
-      </c>
-      <c r="D62" s="2" t="s">
+      <c r="C62" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E62" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="2" t="s">
+      <c r="G62" s="3"/>
+      <c r="H62" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="2" t="s">
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" ht="14.25" customHeight="1">
+      <c r="A63" s="3"/>
+      <c r="B63" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2" t="s">
+      <c r="C63" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E63" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2" t="s">
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" ht="14.25" customHeight="1">
+      <c r="A64" s="3"/>
+      <c r="B64" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
-      <c r="D64" s="2" t="s">
+      <c r="C64" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E64" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F64" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="2" t="s">
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" ht="14.25" customHeight="1">
+      <c r="A65" s="3"/>
+      <c r="B65" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="C65" s="1">
-        <v>12</v>
-      </c>
-      <c r="D65" s="2" t="s">
+      <c r="C65" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="2" t="s">
+      <c r="G65" s="3"/>
+      <c r="H65" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="2" t="s">
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" ht="14.25" customHeight="1">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C66" s="1">
-        <v>1</v>
-      </c>
-      <c r="D66" s="2" t="s">
+      <c r="C66" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="2" t="s">
+      <c r="G66" s="3"/>
+      <c r="H66" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="2" t="s">
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" ht="14.25" customHeight="1">
+      <c r="A67" s="3"/>
+      <c r="B67" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C67" s="1">
-        <v>1</v>
-      </c>
-      <c r="D67" s="2" t="s">
+      <c r="C67" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E67" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="G67" s="1"/>
-      <c r="H67" s="2" t="s">
+      <c r="G67" s="3"/>
+      <c r="H67" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="2" t="s">
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" ht="14.25" customHeight="1">
+      <c r="A68" s="3"/>
+      <c r="B68" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="2" t="s">
+      <c r="C68" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E68" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G68" s="1"/>
-      <c r="H68" s="2" t="s">
+      <c r="G68" s="3"/>
+      <c r="H68" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2" t="s">
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" ht="14.25" customHeight="1">
+      <c r="A69" s="3"/>
+      <c r="B69" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C69" s="1">
-        <v>2</v>
-      </c>
-      <c r="D69" s="1"/>
-      <c r="E69" s="2" t="s">
+      <c r="C69" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G69" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="H69" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="2" t="s">
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="A70" s="3"/>
+      <c r="B70" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C70" s="1">
-        <v>2</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="C70" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E70" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G70" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H70" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="2" t="s">
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="3"/>
+      <c r="B71" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="C71" s="1">
-        <v>1</v>
-      </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="2" t="s">
+      <c r="C71" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D71" s="3"/>
+      <c r="E71" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G71" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="H71" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2" t="s">
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="3"/>
+      <c r="B72" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C72" s="1">
-        <v>1</v>
-      </c>
-      <c r="D72" s="2" t="s">
+      <c r="C72" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E72" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="H72" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="G72" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="2" t="s">
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="A73" s="3"/>
+      <c r="B73" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="C73" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="E73" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="F73" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="G73" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="I73" s="1"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="2" t="s">
+      <c r="H73" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C74" s="1">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2" t="s">
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="A74" s="3"/>
+      <c r="B74" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="C74" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="E74" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="F74" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="G74" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="I74" s="1"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="2" t="s">
+      <c r="H74" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="C75" s="1">
-        <v>1</v>
-      </c>
-      <c r="D75" s="2" t="s">
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" ht="14.25" customHeight="1">
+      <c r="A75" s="3"/>
+      <c r="B75" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="C75" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="G75" s="2" t="s">
+      <c r="E75" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="F75" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="I75" s="1"/>
-    </row>
+      <c r="H75" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
+    <row r="126" ht="14.25" customHeight="1"/>
+    <row r="127" ht="14.25" customHeight="1"/>
+    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="129" ht="14.25" customHeight="1"/>
+    <row r="130" ht="14.25" customHeight="1"/>
+    <row r="131" ht="14.25" customHeight="1"/>
+    <row r="132" ht="14.25" customHeight="1"/>
+    <row r="133" ht="14.25" customHeight="1"/>
+    <row r="134" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1"/>
+    <row r="136" ht="14.25" customHeight="1"/>
+    <row r="137" ht="14.25" customHeight="1"/>
+    <row r="138" ht="14.25" customHeight="1"/>
+    <row r="139" ht="14.25" customHeight="1"/>
+    <row r="140" ht="14.25" customHeight="1"/>
+    <row r="141" ht="14.25" customHeight="1"/>
+    <row r="142" ht="14.25" customHeight="1"/>
+    <row r="143" ht="14.25" customHeight="1"/>
+    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="145" ht="14.25" customHeight="1"/>
+    <row r="146" ht="14.25" customHeight="1"/>
+    <row r="147" ht="14.25" customHeight="1"/>
+    <row r="148" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1"/>
+    <row r="150" ht="14.25" customHeight="1"/>
+    <row r="151" ht="14.25" customHeight="1"/>
+    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="153" ht="14.25" customHeight="1"/>
+    <row r="154" ht="14.25" customHeight="1"/>
+    <row r="155" ht="14.25" customHeight="1"/>
+    <row r="156" ht="14.25" customHeight="1"/>
+    <row r="157" ht="14.25" customHeight="1"/>
+    <row r="158" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1"/>
+    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="161" ht="14.25" customHeight="1"/>
+    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="163" ht="14.25" customHeight="1"/>
+    <row r="164" ht="14.25" customHeight="1"/>
+    <row r="165" ht="14.25" customHeight="1"/>
+    <row r="166" ht="14.25" customHeight="1"/>
+    <row r="167" ht="14.25" customHeight="1"/>
+    <row r="168" ht="14.25" customHeight="1"/>
+    <row r="169" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1"/>
+    <row r="171" ht="14.25" customHeight="1"/>
+    <row r="172" ht="14.25" customHeight="1"/>
+    <row r="173" ht="14.25" customHeight="1"/>
+    <row r="174" ht="14.25" customHeight="1"/>
+    <row r="175" ht="14.25" customHeight="1"/>
+    <row r="176" ht="14.25" customHeight="1"/>
+    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="178" ht="14.25" customHeight="1"/>
+    <row r="179" ht="14.25" customHeight="1"/>
+    <row r="180" ht="14.25" customHeight="1"/>
+    <row r="181" ht="14.25" customHeight="1"/>
+    <row r="182" ht="14.25" customHeight="1"/>
+    <row r="183" ht="14.25" customHeight="1"/>
+    <row r="184" ht="14.25" customHeight="1"/>
+    <row r="185" ht="14.25" customHeight="1"/>
+    <row r="186" ht="14.25" customHeight="1"/>
+    <row r="187" ht="14.25" customHeight="1"/>
+    <row r="188" ht="14.25" customHeight="1"/>
+    <row r="189" ht="14.25" customHeight="1"/>
+    <row r="190" ht="14.25" customHeight="1"/>
+    <row r="191" ht="14.25" customHeight="1"/>
+    <row r="192" ht="14.25" customHeight="1"/>
+    <row r="193" ht="14.25" customHeight="1"/>
+    <row r="194" ht="14.25" customHeight="1"/>
+    <row r="195" ht="14.25" customHeight="1"/>
+    <row r="196" ht="14.25" customHeight="1"/>
+    <row r="197" ht="14.25" customHeight="1"/>
+    <row r="198" ht="14.25" customHeight="1"/>
+    <row r="199" ht="14.25" customHeight="1"/>
+    <row r="200" ht="14.25" customHeight="1"/>
+    <row r="201" ht="14.25" customHeight="1"/>
+    <row r="202" ht="14.25" customHeight="1"/>
+    <row r="203" ht="14.25" customHeight="1"/>
+    <row r="204" ht="14.25" customHeight="1"/>
+    <row r="205" ht="14.25" customHeight="1"/>
+    <row r="206" ht="14.25" customHeight="1"/>
+    <row r="207" ht="14.25" customHeight="1"/>
+    <row r="208" ht="14.25" customHeight="1"/>
+    <row r="209" ht="14.25" customHeight="1"/>
+    <row r="210" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1"/>
+    <row r="212" ht="14.25" customHeight="1"/>
+    <row r="213" ht="14.25" customHeight="1"/>
+    <row r="214" ht="14.25" customHeight="1"/>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
+    <row r="218" ht="14.25" customHeight="1"/>
+    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="221" ht="14.25" customHeight="1"/>
+    <row r="222" ht="14.25" customHeight="1"/>
+    <row r="223" ht="14.25" customHeight="1"/>
+    <row r="224" ht="14.25" customHeight="1"/>
+    <row r="225" ht="14.25" customHeight="1"/>
+    <row r="226" ht="14.25" customHeight="1"/>
+    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1"/>
+    <row r="229" ht="14.25" customHeight="1"/>
+    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="231" ht="14.25" customHeight="1"/>
+    <row r="232" ht="14.25" customHeight="1"/>
+    <row r="233" ht="14.25" customHeight="1"/>
+    <row r="234" ht="14.25" customHeight="1"/>
+    <row r="235" ht="14.25" customHeight="1"/>
+    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="237" ht="14.25" customHeight="1"/>
+    <row r="238" ht="14.25" customHeight="1"/>
+    <row r="239" ht="14.25" customHeight="1"/>
+    <row r="240" ht="14.25" customHeight="1"/>
+    <row r="241" ht="14.25" customHeight="1"/>
+    <row r="242" ht="14.25" customHeight="1"/>
+    <row r="243" ht="14.25" customHeight="1"/>
+    <row r="244" ht="14.25" customHeight="1"/>
+    <row r="245" ht="14.25" customHeight="1"/>
+    <row r="246" ht="14.25" customHeight="1"/>
+    <row r="247" ht="14.25" customHeight="1"/>
+    <row r="248" ht="14.25" customHeight="1"/>
+    <row r="249" ht="14.25" customHeight="1"/>
+    <row r="250" ht="14.25" customHeight="1"/>
+    <row r="251" ht="14.25" customHeight="1"/>
+    <row r="252" ht="14.25" customHeight="1"/>
+    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="254" ht="14.25" customHeight="1"/>
+    <row r="255" ht="14.25" customHeight="1"/>
+    <row r="256" ht="14.25" customHeight="1"/>
+    <row r="257" ht="14.25" customHeight="1"/>
+    <row r="258" ht="14.25" customHeight="1"/>
+    <row r="259" ht="14.25" customHeight="1"/>
+    <row r="260" ht="14.25" customHeight="1"/>
+    <row r="261" ht="14.25" customHeight="1"/>
+    <row r="262" ht="14.25" customHeight="1"/>
+    <row r="263" ht="14.25" customHeight="1"/>
+    <row r="264" ht="14.25" customHeight="1"/>
+    <row r="265" ht="14.25" customHeight="1"/>
+    <row r="266" ht="14.25" customHeight="1"/>
+    <row r="267" ht="14.25" customHeight="1"/>
+    <row r="268" ht="14.25" customHeight="1"/>
+    <row r="269" ht="14.25" customHeight="1"/>
+    <row r="270" ht="14.25" customHeight="1"/>
+    <row r="271" ht="14.25" customHeight="1"/>
+    <row r="272" ht="14.25" customHeight="1"/>
+    <row r="273" ht="14.25" customHeight="1"/>
+    <row r="274" ht="14.25" customHeight="1"/>
+    <row r="275" ht="14.25" customHeight="1"/>
+    <row r="276" ht="14.25" customHeight="1"/>
+    <row r="277" ht="14.25" customHeight="1"/>
+    <row r="278" ht="14.25" customHeight="1"/>
+    <row r="279" ht="14.25" customHeight="1"/>
+    <row r="280" ht="14.25" customHeight="1"/>
+    <row r="281" ht="14.25" customHeight="1"/>
+    <row r="282" ht="14.25" customHeight="1"/>
+    <row r="283" ht="14.25" customHeight="1"/>
+    <row r="284" ht="14.25" customHeight="1"/>
+    <row r="285" ht="14.25" customHeight="1"/>
+    <row r="286" ht="14.25" customHeight="1"/>
+    <row r="287" ht="14.25" customHeight="1"/>
+    <row r="288" ht="14.25" customHeight="1"/>
+    <row r="289" ht="14.25" customHeight="1"/>
+    <row r="290" ht="14.25" customHeight="1"/>
+    <row r="291" ht="14.25" customHeight="1"/>
+    <row r="292" ht="14.25" customHeight="1"/>
+    <row r="293" ht="14.25" customHeight="1"/>
+    <row r="294" ht="14.25" customHeight="1"/>
+    <row r="295" ht="14.25" customHeight="1"/>
+    <row r="296" ht="14.25" customHeight="1"/>
+    <row r="297" ht="14.25" customHeight="1"/>
+    <row r="298" ht="14.25" customHeight="1"/>
+    <row r="299" ht="14.25" customHeight="1"/>
+    <row r="300" ht="14.25" customHeight="1"/>
+    <row r="301" ht="14.25" customHeight="1"/>
+    <row r="302" ht="14.25" customHeight="1"/>
+    <row r="303" ht="14.25" customHeight="1"/>
+    <row r="304" ht="14.25" customHeight="1"/>
+    <row r="305" ht="14.25" customHeight="1"/>
+    <row r="306" ht="14.25" customHeight="1"/>
+    <row r="307" ht="14.25" customHeight="1"/>
+    <row r="308" ht="14.25" customHeight="1"/>
+    <row r="309" ht="14.25" customHeight="1"/>
+    <row r="310" ht="14.25" customHeight="1"/>
+    <row r="311" ht="14.25" customHeight="1"/>
+    <row r="312" ht="14.25" customHeight="1"/>
+    <row r="313" ht="14.25" customHeight="1"/>
+    <row r="314" ht="14.25" customHeight="1"/>
+    <row r="315" ht="14.25" customHeight="1"/>
+    <row r="316" ht="14.25" customHeight="1"/>
+    <row r="317" ht="14.25" customHeight="1"/>
+    <row r="318" ht="14.25" customHeight="1"/>
+    <row r="319" ht="14.25" customHeight="1"/>
+    <row r="320" ht="14.25" customHeight="1"/>
+    <row r="321" ht="14.25" customHeight="1"/>
+    <row r="322" ht="14.25" customHeight="1"/>
+    <row r="323" ht="14.25" customHeight="1"/>
+    <row r="324" ht="14.25" customHeight="1"/>
+    <row r="325" ht="14.25" customHeight="1"/>
+    <row r="326" ht="14.25" customHeight="1"/>
+    <row r="327" ht="14.25" customHeight="1"/>
+    <row r="328" ht="14.25" customHeight="1"/>
+    <row r="329" ht="14.25" customHeight="1"/>
+    <row r="330" ht="14.25" customHeight="1"/>
+    <row r="331" ht="14.25" customHeight="1"/>
+    <row r="332" ht="14.25" customHeight="1"/>
+    <row r="333" ht="14.25" customHeight="1"/>
+    <row r="334" ht="14.25" customHeight="1"/>
+    <row r="335" ht="14.25" customHeight="1"/>
+    <row r="336" ht="14.25" customHeight="1"/>
+    <row r="337" ht="14.25" customHeight="1"/>
+    <row r="338" ht="14.25" customHeight="1"/>
+    <row r="339" ht="14.25" customHeight="1"/>
+    <row r="340" ht="14.25" customHeight="1"/>
+    <row r="341" ht="14.25" customHeight="1"/>
+    <row r="342" ht="14.25" customHeight="1"/>
+    <row r="343" ht="14.25" customHeight="1"/>
+    <row r="344" ht="14.25" customHeight="1"/>
+    <row r="345" ht="14.25" customHeight="1"/>
+    <row r="346" ht="14.25" customHeight="1"/>
+    <row r="347" ht="14.25" customHeight="1"/>
+    <row r="348" ht="14.25" customHeight="1"/>
+    <row r="349" ht="14.25" customHeight="1"/>
+    <row r="350" ht="14.25" customHeight="1"/>
+    <row r="351" ht="14.25" customHeight="1"/>
+    <row r="352" ht="14.25" customHeight="1"/>
+    <row r="353" ht="14.25" customHeight="1"/>
+    <row r="354" ht="14.25" customHeight="1"/>
+    <row r="355" ht="14.25" customHeight="1"/>
+    <row r="356" ht="14.25" customHeight="1"/>
+    <row r="357" ht="14.25" customHeight="1"/>
+    <row r="358" ht="14.25" customHeight="1"/>
+    <row r="359" ht="14.25" customHeight="1"/>
+    <row r="360" ht="14.25" customHeight="1"/>
+    <row r="361" ht="14.25" customHeight="1"/>
+    <row r="362" ht="14.25" customHeight="1"/>
+    <row r="363" ht="14.25" customHeight="1"/>
+    <row r="364" ht="14.25" customHeight="1"/>
+    <row r="365" ht="14.25" customHeight="1"/>
+    <row r="366" ht="14.25" customHeight="1"/>
+    <row r="367" ht="14.25" customHeight="1"/>
+    <row r="368" ht="14.25" customHeight="1"/>
+    <row r="369" ht="14.25" customHeight="1"/>
+    <row r="370" ht="14.25" customHeight="1"/>
+    <row r="371" ht="14.25" customHeight="1"/>
+    <row r="372" ht="14.25" customHeight="1"/>
+    <row r="373" ht="14.25" customHeight="1"/>
+    <row r="374" ht="14.25" customHeight="1"/>
+    <row r="375" ht="14.25" customHeight="1"/>
+    <row r="376" ht="14.25" customHeight="1"/>
+    <row r="377" ht="14.25" customHeight="1"/>
+    <row r="378" ht="14.25" customHeight="1"/>
+    <row r="379" ht="14.25" customHeight="1"/>
+    <row r="380" ht="14.25" customHeight="1"/>
+    <row r="381" ht="14.25" customHeight="1"/>
+    <row r="382" ht="14.25" customHeight="1"/>
+    <row r="383" ht="14.25" customHeight="1"/>
+    <row r="384" ht="14.25" customHeight="1"/>
+    <row r="385" ht="14.25" customHeight="1"/>
+    <row r="386" ht="14.25" customHeight="1"/>
+    <row r="387" ht="14.25" customHeight="1"/>
+    <row r="388" ht="14.25" customHeight="1"/>
+    <row r="389" ht="14.25" customHeight="1"/>
+    <row r="390" ht="14.25" customHeight="1"/>
+    <row r="391" ht="14.25" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1"/>
+    <row r="393" ht="14.25" customHeight="1"/>
+    <row r="394" ht="14.25" customHeight="1"/>
+    <row r="395" ht="14.25" customHeight="1"/>
+    <row r="396" ht="14.25" customHeight="1"/>
+    <row r="397" ht="14.25" customHeight="1"/>
+    <row r="398" ht="14.25" customHeight="1"/>
+    <row r="399" ht="14.25" customHeight="1"/>
+    <row r="400" ht="14.25" customHeight="1"/>
+    <row r="401" ht="14.25" customHeight="1"/>
+    <row r="402" ht="14.25" customHeight="1"/>
+    <row r="403" ht="14.25" customHeight="1"/>
+    <row r="404" ht="14.25" customHeight="1"/>
+    <row r="405" ht="14.25" customHeight="1"/>
+    <row r="406" ht="14.25" customHeight="1"/>
+    <row r="407" ht="14.25" customHeight="1"/>
+    <row r="408" ht="14.25" customHeight="1"/>
+    <row r="409" ht="14.25" customHeight="1"/>
+    <row r="410" ht="14.25" customHeight="1"/>
+    <row r="411" ht="14.25" customHeight="1"/>
+    <row r="412" ht="14.25" customHeight="1"/>
+    <row r="413" ht="14.25" customHeight="1"/>
+    <row r="414" ht="14.25" customHeight="1"/>
+    <row r="415" ht="14.25" customHeight="1"/>
+    <row r="416" ht="14.25" customHeight="1"/>
+    <row r="417" ht="14.25" customHeight="1"/>
+    <row r="418" ht="14.25" customHeight="1"/>
+    <row r="419" ht="14.25" customHeight="1"/>
+    <row r="420" ht="14.25" customHeight="1"/>
+    <row r="421" ht="14.25" customHeight="1"/>
+    <row r="422" ht="14.25" customHeight="1"/>
+    <row r="423" ht="14.25" customHeight="1"/>
+    <row r="424" ht="14.25" customHeight="1"/>
+    <row r="425" ht="14.25" customHeight="1"/>
+    <row r="426" ht="14.25" customHeight="1"/>
+    <row r="427" ht="14.25" customHeight="1"/>
+    <row r="428" ht="14.25" customHeight="1"/>
+    <row r="429" ht="14.25" customHeight="1"/>
+    <row r="430" ht="14.25" customHeight="1"/>
+    <row r="431" ht="14.25" customHeight="1"/>
+    <row r="432" ht="14.25" customHeight="1"/>
+    <row r="433" ht="14.25" customHeight="1"/>
+    <row r="434" ht="14.25" customHeight="1"/>
+    <row r="435" ht="14.25" customHeight="1"/>
+    <row r="436" ht="14.25" customHeight="1"/>
+    <row r="437" ht="14.25" customHeight="1"/>
+    <row r="438" ht="14.25" customHeight="1"/>
+    <row r="439" ht="14.25" customHeight="1"/>
+    <row r="440" ht="14.25" customHeight="1"/>
+    <row r="441" ht="14.25" customHeight="1"/>
+    <row r="442" ht="14.25" customHeight="1"/>
+    <row r="443" ht="14.25" customHeight="1"/>
+    <row r="444" ht="14.25" customHeight="1"/>
+    <row r="445" ht="14.25" customHeight="1"/>
+    <row r="446" ht="14.25" customHeight="1"/>
+    <row r="447" ht="14.25" customHeight="1"/>
+    <row r="448" ht="14.25" customHeight="1"/>
+    <row r="449" ht="14.25" customHeight="1"/>
+    <row r="450" ht="14.25" customHeight="1"/>
+    <row r="451" ht="14.25" customHeight="1"/>
+    <row r="452" ht="14.25" customHeight="1"/>
+    <row r="453" ht="14.25" customHeight="1"/>
+    <row r="454" ht="14.25" customHeight="1"/>
+    <row r="455" ht="14.25" customHeight="1"/>
+    <row r="456" ht="14.25" customHeight="1"/>
+    <row r="457" ht="14.25" customHeight="1"/>
+    <row r="458" ht="14.25" customHeight="1"/>
+    <row r="459" ht="14.25" customHeight="1"/>
+    <row r="460" ht="14.25" customHeight="1"/>
+    <row r="461" ht="14.25" customHeight="1"/>
+    <row r="462" ht="14.25" customHeight="1"/>
+    <row r="463" ht="14.25" customHeight="1"/>
+    <row r="464" ht="14.25" customHeight="1"/>
+    <row r="465" ht="14.25" customHeight="1"/>
+    <row r="466" ht="14.25" customHeight="1"/>
+    <row r="467" ht="14.25" customHeight="1"/>
+    <row r="468" ht="14.25" customHeight="1"/>
+    <row r="469" ht="14.25" customHeight="1"/>
+    <row r="470" ht="14.25" customHeight="1"/>
+    <row r="471" ht="14.25" customHeight="1"/>
+    <row r="472" ht="14.25" customHeight="1"/>
+    <row r="473" ht="14.25" customHeight="1"/>
+    <row r="474" ht="14.25" customHeight="1"/>
+    <row r="475" ht="14.25" customHeight="1"/>
+    <row r="476" ht="14.25" customHeight="1"/>
+    <row r="477" ht="14.25" customHeight="1"/>
+    <row r="478" ht="14.25" customHeight="1"/>
+    <row r="479" ht="14.25" customHeight="1"/>
+    <row r="480" ht="14.25" customHeight="1"/>
+    <row r="481" ht="14.25" customHeight="1"/>
+    <row r="482" ht="14.25" customHeight="1"/>
+    <row r="483" ht="14.25" customHeight="1"/>
+    <row r="484" ht="14.25" customHeight="1"/>
+    <row r="485" ht="14.25" customHeight="1"/>
+    <row r="486" ht="14.25" customHeight="1"/>
+    <row r="487" ht="14.25" customHeight="1"/>
+    <row r="488" ht="14.25" customHeight="1"/>
+    <row r="489" ht="14.25" customHeight="1"/>
+    <row r="490" ht="14.25" customHeight="1"/>
+    <row r="491" ht="14.25" customHeight="1"/>
+    <row r="492" ht="14.25" customHeight="1"/>
+    <row r="493" ht="14.25" customHeight="1"/>
+    <row r="494" ht="14.25" customHeight="1"/>
+    <row r="495" ht="14.25" customHeight="1"/>
+    <row r="496" ht="14.25" customHeight="1"/>
+    <row r="497" ht="14.25" customHeight="1"/>
+    <row r="498" ht="14.25" customHeight="1"/>
+    <row r="499" ht="14.25" customHeight="1"/>
+    <row r="500" ht="14.25" customHeight="1"/>
+    <row r="501" ht="14.25" customHeight="1"/>
+    <row r="502" ht="14.25" customHeight="1"/>
+    <row r="503" ht="14.25" customHeight="1"/>
+    <row r="504" ht="14.25" customHeight="1"/>
+    <row r="505" ht="14.25" customHeight="1"/>
+    <row r="506" ht="14.25" customHeight="1"/>
+    <row r="507" ht="14.25" customHeight="1"/>
+    <row r="508" ht="14.25" customHeight="1"/>
+    <row r="509" ht="14.25" customHeight="1"/>
+    <row r="510" ht="14.25" customHeight="1"/>
+    <row r="511" ht="14.25" customHeight="1"/>
+    <row r="512" ht="14.25" customHeight="1"/>
+    <row r="513" ht="14.25" customHeight="1"/>
+    <row r="514" ht="14.25" customHeight="1"/>
+    <row r="515" ht="14.25" customHeight="1"/>
+    <row r="516" ht="14.25" customHeight="1"/>
+    <row r="517" ht="14.25" customHeight="1"/>
+    <row r="518" ht="14.25" customHeight="1"/>
+    <row r="519" ht="14.25" customHeight="1"/>
+    <row r="520" ht="14.25" customHeight="1"/>
+    <row r="521" ht="14.25" customHeight="1"/>
+    <row r="522" ht="14.25" customHeight="1"/>
+    <row r="523" ht="14.25" customHeight="1"/>
+    <row r="524" ht="14.25" customHeight="1"/>
+    <row r="525" ht="14.25" customHeight="1"/>
+    <row r="526" ht="14.25" customHeight="1"/>
+    <row r="527" ht="14.25" customHeight="1"/>
+    <row r="528" ht="14.25" customHeight="1"/>
+    <row r="529" ht="14.25" customHeight="1"/>
+    <row r="530" ht="14.25" customHeight="1"/>
+    <row r="531" ht="14.25" customHeight="1"/>
+    <row r="532" ht="14.25" customHeight="1"/>
+    <row r="533" ht="14.25" customHeight="1"/>
+    <row r="534" ht="14.25" customHeight="1"/>
+    <row r="535" ht="14.25" customHeight="1"/>
+    <row r="536" ht="14.25" customHeight="1"/>
+    <row r="537" ht="14.25" customHeight="1"/>
+    <row r="538" ht="14.25" customHeight="1"/>
+    <row r="539" ht="14.25" customHeight="1"/>
+    <row r="540" ht="14.25" customHeight="1"/>
+    <row r="541" ht="14.25" customHeight="1"/>
+    <row r="542" ht="14.25" customHeight="1"/>
+    <row r="543" ht="14.25" customHeight="1"/>
+    <row r="544" ht="14.25" customHeight="1"/>
+    <row r="545" ht="14.25" customHeight="1"/>
+    <row r="546" ht="14.25" customHeight="1"/>
+    <row r="547" ht="14.25" customHeight="1"/>
+    <row r="548" ht="14.25" customHeight="1"/>
+    <row r="549" ht="14.25" customHeight="1"/>
+    <row r="550" ht="14.25" customHeight="1"/>
+    <row r="551" ht="14.25" customHeight="1"/>
+    <row r="552" ht="14.25" customHeight="1"/>
+    <row r="553" ht="14.25" customHeight="1"/>
+    <row r="554" ht="14.25" customHeight="1"/>
+    <row r="555" ht="14.25" customHeight="1"/>
+    <row r="556" ht="14.25" customHeight="1"/>
+    <row r="557" ht="14.25" customHeight="1"/>
+    <row r="558" ht="14.25" customHeight="1"/>
+    <row r="559" ht="14.25" customHeight="1"/>
+    <row r="560" ht="14.25" customHeight="1"/>
+    <row r="561" ht="14.25" customHeight="1"/>
+    <row r="562" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1"/>
+    <row r="564" ht="14.25" customHeight="1"/>
+    <row r="565" ht="14.25" customHeight="1"/>
+    <row r="566" ht="14.25" customHeight="1"/>
+    <row r="567" ht="14.25" customHeight="1"/>
+    <row r="568" ht="14.25" customHeight="1"/>
+    <row r="569" ht="14.25" customHeight="1"/>
+    <row r="570" ht="14.25" customHeight="1"/>
+    <row r="571" ht="14.25" customHeight="1"/>
+    <row r="572" ht="14.25" customHeight="1"/>
+    <row r="573" ht="14.25" customHeight="1"/>
+    <row r="574" ht="14.25" customHeight="1"/>
+    <row r="575" ht="14.25" customHeight="1"/>
+    <row r="576" ht="14.25" customHeight="1"/>
+    <row r="577" ht="14.25" customHeight="1"/>
+    <row r="578" ht="14.25" customHeight="1"/>
+    <row r="579" ht="14.25" customHeight="1"/>
+    <row r="580" ht="14.25" customHeight="1"/>
+    <row r="581" ht="14.25" customHeight="1"/>
+    <row r="582" ht="14.25" customHeight="1"/>
+    <row r="583" ht="14.25" customHeight="1"/>
+    <row r="584" ht="14.25" customHeight="1"/>
+    <row r="585" ht="14.25" customHeight="1"/>
+    <row r="586" ht="14.25" customHeight="1"/>
+    <row r="587" ht="14.25" customHeight="1"/>
+    <row r="588" ht="14.25" customHeight="1"/>
+    <row r="589" ht="14.25" customHeight="1"/>
+    <row r="590" ht="14.25" customHeight="1"/>
+    <row r="591" ht="14.25" customHeight="1"/>
+    <row r="592" ht="14.25" customHeight="1"/>
+    <row r="593" ht="14.25" customHeight="1"/>
+    <row r="594" ht="14.25" customHeight="1"/>
+    <row r="595" ht="14.25" customHeight="1"/>
+    <row r="596" ht="14.25" customHeight="1"/>
+    <row r="597" ht="14.25" customHeight="1"/>
+    <row r="598" ht="14.25" customHeight="1"/>
+    <row r="599" ht="14.25" customHeight="1"/>
+    <row r="600" ht="14.25" customHeight="1"/>
+    <row r="601" ht="14.25" customHeight="1"/>
+    <row r="602" ht="14.25" customHeight="1"/>
+    <row r="603" ht="14.25" customHeight="1"/>
+    <row r="604" ht="14.25" customHeight="1"/>
+    <row r="605" ht="14.25" customHeight="1"/>
+    <row r="606" ht="14.25" customHeight="1"/>
+    <row r="607" ht="14.25" customHeight="1"/>
+    <row r="608" ht="14.25" customHeight="1"/>
+    <row r="609" ht="14.25" customHeight="1"/>
+    <row r="610" ht="14.25" customHeight="1"/>
+    <row r="611" ht="14.25" customHeight="1"/>
+    <row r="612" ht="14.25" customHeight="1"/>
+    <row r="613" ht="14.25" customHeight="1"/>
+    <row r="614" ht="14.25" customHeight="1"/>
+    <row r="615" ht="14.25" customHeight="1"/>
+    <row r="616" ht="14.25" customHeight="1"/>
+    <row r="617" ht="14.25" customHeight="1"/>
+    <row r="618" ht="14.25" customHeight="1"/>
+    <row r="619" ht="14.25" customHeight="1"/>
+    <row r="620" ht="14.25" customHeight="1"/>
+    <row r="621" ht="14.25" customHeight="1"/>
+    <row r="622" ht="14.25" customHeight="1"/>
+    <row r="623" ht="14.25" customHeight="1"/>
+    <row r="624" ht="14.25" customHeight="1"/>
+    <row r="625" ht="14.25" customHeight="1"/>
+    <row r="626" ht="14.25" customHeight="1"/>
+    <row r="627" ht="14.25" customHeight="1"/>
+    <row r="628" ht="14.25" customHeight="1"/>
+    <row r="629" ht="14.25" customHeight="1"/>
+    <row r="630" ht="14.25" customHeight="1"/>
+    <row r="631" ht="14.25" customHeight="1"/>
+    <row r="632" ht="14.25" customHeight="1"/>
+    <row r="633" ht="14.25" customHeight="1"/>
+    <row r="634" ht="14.25" customHeight="1"/>
+    <row r="635" ht="14.25" customHeight="1"/>
+    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="637" ht="14.25" customHeight="1"/>
+    <row r="638" ht="14.25" customHeight="1"/>
+    <row r="639" ht="14.25" customHeight="1"/>
+    <row r="640" ht="14.25" customHeight="1"/>
+    <row r="641" ht="14.25" customHeight="1"/>
+    <row r="642" ht="14.25" customHeight="1"/>
+    <row r="643" ht="14.25" customHeight="1"/>
+    <row r="644" ht="14.25" customHeight="1"/>
+    <row r="645" ht="14.25" customHeight="1"/>
+    <row r="646" ht="14.25" customHeight="1"/>
+    <row r="647" ht="14.25" customHeight="1"/>
+    <row r="648" ht="14.25" customHeight="1"/>
+    <row r="649" ht="14.25" customHeight="1"/>
+    <row r="650" ht="14.25" customHeight="1"/>
+    <row r="651" ht="14.25" customHeight="1"/>
+    <row r="652" ht="14.25" customHeight="1"/>
+    <row r="653" ht="14.25" customHeight="1"/>
+    <row r="654" ht="14.25" customHeight="1"/>
+    <row r="655" ht="14.25" customHeight="1"/>
+    <row r="656" ht="14.25" customHeight="1"/>
+    <row r="657" ht="14.25" customHeight="1"/>
+    <row r="658" ht="14.25" customHeight="1"/>
+    <row r="659" ht="14.25" customHeight="1"/>
+    <row r="660" ht="14.25" customHeight="1"/>
+    <row r="661" ht="14.25" customHeight="1"/>
+    <row r="662" ht="14.25" customHeight="1"/>
+    <row r="663" ht="14.25" customHeight="1"/>
+    <row r="664" ht="14.25" customHeight="1"/>
+    <row r="665" ht="14.25" customHeight="1"/>
+    <row r="666" ht="14.25" customHeight="1"/>
+    <row r="667" ht="14.25" customHeight="1"/>
+    <row r="668" ht="14.25" customHeight="1"/>
+    <row r="669" ht="14.25" customHeight="1"/>
+    <row r="670" ht="14.25" customHeight="1"/>
+    <row r="671" ht="14.25" customHeight="1"/>
+    <row r="672" ht="14.25" customHeight="1"/>
+    <row r="673" ht="14.25" customHeight="1"/>
+    <row r="674" ht="14.25" customHeight="1"/>
+    <row r="675" ht="14.25" customHeight="1"/>
+    <row r="676" ht="14.25" customHeight="1"/>
+    <row r="677" ht="14.25" customHeight="1"/>
+    <row r="678" ht="14.25" customHeight="1"/>
+    <row r="679" ht="14.25" customHeight="1"/>
+    <row r="680" ht="14.25" customHeight="1"/>
+    <row r="681" ht="14.25" customHeight="1"/>
+    <row r="682" ht="14.25" customHeight="1"/>
+    <row r="683" ht="14.25" customHeight="1"/>
+    <row r="684" ht="14.25" customHeight="1"/>
+    <row r="685" ht="14.25" customHeight="1"/>
+    <row r="686" ht="14.25" customHeight="1"/>
+    <row r="687" ht="14.25" customHeight="1"/>
+    <row r="688" ht="14.25" customHeight="1"/>
+    <row r="689" ht="14.25" customHeight="1"/>
+    <row r="690" ht="14.25" customHeight="1"/>
+    <row r="691" ht="14.25" customHeight="1"/>
+    <row r="692" ht="14.25" customHeight="1"/>
+    <row r="693" ht="14.25" customHeight="1"/>
+    <row r="694" ht="14.25" customHeight="1"/>
+    <row r="695" ht="14.25" customHeight="1"/>
+    <row r="696" ht="14.25" customHeight="1"/>
+    <row r="697" ht="14.25" customHeight="1"/>
+    <row r="698" ht="14.25" customHeight="1"/>
+    <row r="699" ht="14.25" customHeight="1"/>
+    <row r="700" ht="14.25" customHeight="1"/>
+    <row r="701" ht="14.25" customHeight="1"/>
+    <row r="702" ht="14.25" customHeight="1"/>
+    <row r="703" ht="14.25" customHeight="1"/>
+    <row r="704" ht="14.25" customHeight="1"/>
+    <row r="705" ht="14.25" customHeight="1"/>
+    <row r="706" ht="14.25" customHeight="1"/>
+    <row r="707" ht="14.25" customHeight="1"/>
+    <row r="708" ht="14.25" customHeight="1"/>
+    <row r="709" ht="14.25" customHeight="1"/>
+    <row r="710" ht="14.25" customHeight="1"/>
+    <row r="711" ht="14.25" customHeight="1"/>
+    <row r="712" ht="14.25" customHeight="1"/>
+    <row r="713" ht="14.25" customHeight="1"/>
+    <row r="714" ht="14.25" customHeight="1"/>
+    <row r="715" ht="14.25" customHeight="1"/>
+    <row r="716" ht="14.25" customHeight="1"/>
+    <row r="717" ht="14.25" customHeight="1"/>
+    <row r="718" ht="14.25" customHeight="1"/>
+    <row r="719" ht="14.25" customHeight="1"/>
+    <row r="720" ht="14.25" customHeight="1"/>
+    <row r="721" ht="14.25" customHeight="1"/>
+    <row r="722" ht="14.25" customHeight="1"/>
+    <row r="723" ht="14.25" customHeight="1"/>
+    <row r="724" ht="14.25" customHeight="1"/>
+    <row r="725" ht="14.25" customHeight="1"/>
+    <row r="726" ht="14.25" customHeight="1"/>
+    <row r="727" ht="14.25" customHeight="1"/>
+    <row r="728" ht="14.25" customHeight="1"/>
+    <row r="729" ht="14.25" customHeight="1"/>
+    <row r="730" ht="14.25" customHeight="1"/>
+    <row r="731" ht="14.25" customHeight="1"/>
+    <row r="732" ht="14.25" customHeight="1"/>
+    <row r="733" ht="14.25" customHeight="1"/>
+    <row r="734" ht="14.25" customHeight="1"/>
+    <row r="735" ht="14.25" customHeight="1"/>
+    <row r="736" ht="14.25" customHeight="1"/>
+    <row r="737" ht="14.25" customHeight="1"/>
+    <row r="738" ht="14.25" customHeight="1"/>
+    <row r="739" ht="14.25" customHeight="1"/>
+    <row r="740" ht="14.25" customHeight="1"/>
+    <row r="741" ht="14.25" customHeight="1"/>
+    <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
+    <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
+    <row r="752" ht="14.25" customHeight="1"/>
+    <row r="753" ht="14.25" customHeight="1"/>
+    <row r="754" ht="14.25" customHeight="1"/>
+    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="756" ht="14.25" customHeight="1"/>
+    <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
+    <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
+    <row r="790" ht="14.25" customHeight="1"/>
+    <row r="791" ht="14.25" customHeight="1"/>
+    <row r="792" ht="14.25" customHeight="1"/>
+    <row r="793" ht="14.25" customHeight="1"/>
+    <row r="794" ht="14.25" customHeight="1"/>
+    <row r="795" ht="14.25" customHeight="1"/>
+    <row r="796" ht="14.25" customHeight="1"/>
+    <row r="797" ht="14.25" customHeight="1"/>
+    <row r="798" ht="14.25" customHeight="1"/>
+    <row r="799" ht="14.25" customHeight="1"/>
+    <row r="800" ht="14.25" customHeight="1"/>
+    <row r="801" ht="14.25" customHeight="1"/>
+    <row r="802" ht="14.25" customHeight="1"/>
+    <row r="803" ht="14.25" customHeight="1"/>
+    <row r="804" ht="14.25" customHeight="1"/>
+    <row r="805" ht="14.25" customHeight="1"/>
+    <row r="806" ht="14.25" customHeight="1"/>
+    <row r="807" ht="14.25" customHeight="1"/>
+    <row r="808" ht="14.25" customHeight="1"/>
+    <row r="809" ht="14.25" customHeight="1"/>
+    <row r="810" ht="14.25" customHeight="1"/>
+    <row r="811" ht="14.25" customHeight="1"/>
+    <row r="812" ht="14.25" customHeight="1"/>
+    <row r="813" ht="14.25" customHeight="1"/>
+    <row r="814" ht="14.25" customHeight="1"/>
+    <row r="815" ht="14.25" customHeight="1"/>
+    <row r="816" ht="14.25" customHeight="1"/>
+    <row r="817" ht="14.25" customHeight="1"/>
+    <row r="818" ht="14.25" customHeight="1"/>
+    <row r="819" ht="14.25" customHeight="1"/>
+    <row r="820" ht="14.25" customHeight="1"/>
+    <row r="821" ht="14.25" customHeight="1"/>
+    <row r="822" ht="14.25" customHeight="1"/>
+    <row r="823" ht="14.25" customHeight="1"/>
+    <row r="824" ht="14.25" customHeight="1"/>
+    <row r="825" ht="14.25" customHeight="1"/>
+    <row r="826" ht="14.25" customHeight="1"/>
+    <row r="827" ht="14.25" customHeight="1"/>
+    <row r="828" ht="14.25" customHeight="1"/>
+    <row r="829" ht="14.25" customHeight="1"/>
+    <row r="830" ht="14.25" customHeight="1"/>
+    <row r="831" ht="14.25" customHeight="1"/>
+    <row r="832" ht="14.25" customHeight="1"/>
+    <row r="833" ht="14.25" customHeight="1"/>
+    <row r="834" ht="14.25" customHeight="1"/>
+    <row r="835" ht="14.25" customHeight="1"/>
+    <row r="836" ht="14.25" customHeight="1"/>
+    <row r="837" ht="14.25" customHeight="1"/>
+    <row r="838" ht="14.25" customHeight="1"/>
+    <row r="839" ht="14.25" customHeight="1"/>
+    <row r="840" ht="14.25" customHeight="1"/>
+    <row r="841" ht="14.25" customHeight="1"/>
+    <row r="842" ht="14.25" customHeight="1"/>
+    <row r="843" ht="14.25" customHeight="1"/>
+    <row r="844" ht="14.25" customHeight="1"/>
+    <row r="845" ht="14.25" customHeight="1"/>
+    <row r="846" ht="14.25" customHeight="1"/>
+    <row r="847" ht="14.25" customHeight="1"/>
+    <row r="848" ht="14.25" customHeight="1"/>
+    <row r="849" ht="14.25" customHeight="1"/>
+    <row r="850" ht="14.25" customHeight="1"/>
+    <row r="851" ht="14.25" customHeight="1"/>
+    <row r="852" ht="14.25" customHeight="1"/>
+    <row r="853" ht="14.25" customHeight="1"/>
+    <row r="854" ht="14.25" customHeight="1"/>
+    <row r="855" ht="14.25" customHeight="1"/>
+    <row r="856" ht="14.25" customHeight="1"/>
+    <row r="857" ht="14.25" customHeight="1"/>
+    <row r="858" ht="14.25" customHeight="1"/>
+    <row r="859" ht="14.25" customHeight="1"/>
+    <row r="860" ht="14.25" customHeight="1"/>
+    <row r="861" ht="14.25" customHeight="1"/>
+    <row r="862" ht="14.25" customHeight="1"/>
+    <row r="863" ht="14.25" customHeight="1"/>
+    <row r="864" ht="14.25" customHeight="1"/>
+    <row r="865" ht="14.25" customHeight="1"/>
+    <row r="866" ht="14.25" customHeight="1"/>
+    <row r="867" ht="14.25" customHeight="1"/>
+    <row r="868" ht="14.25" customHeight="1"/>
+    <row r="869" ht="14.25" customHeight="1"/>
+    <row r="870" ht="14.25" customHeight="1"/>
+    <row r="871" ht="14.25" customHeight="1"/>
+    <row r="872" ht="14.25" customHeight="1"/>
+    <row r="873" ht="14.25" customHeight="1"/>
+    <row r="874" ht="14.25" customHeight="1"/>
+    <row r="875" ht="14.25" customHeight="1"/>
+    <row r="876" ht="14.25" customHeight="1"/>
+    <row r="877" ht="14.25" customHeight="1"/>
+    <row r="878" ht="14.25" customHeight="1"/>
+    <row r="879" ht="14.25" customHeight="1"/>
+    <row r="880" ht="14.25" customHeight="1"/>
+    <row r="881" ht="14.25" customHeight="1"/>
+    <row r="882" ht="14.25" customHeight="1"/>
+    <row r="883" ht="14.25" customHeight="1"/>
+    <row r="884" ht="14.25" customHeight="1"/>
+    <row r="885" ht="14.25" customHeight="1"/>
+    <row r="886" ht="14.25" customHeight="1"/>
+    <row r="887" ht="14.25" customHeight="1"/>
+    <row r="888" ht="14.25" customHeight="1"/>
+    <row r="889" ht="14.25" customHeight="1"/>
+    <row r="890" ht="14.25" customHeight="1"/>
+    <row r="891" ht="14.25" customHeight="1"/>
+    <row r="892" ht="14.25" customHeight="1"/>
+    <row r="893" ht="14.25" customHeight="1"/>
+    <row r="894" ht="14.25" customHeight="1"/>
+    <row r="895" ht="14.25" customHeight="1"/>
+    <row r="896" ht="14.25" customHeight="1"/>
+    <row r="897" ht="14.25" customHeight="1"/>
+    <row r="898" ht="14.25" customHeight="1"/>
+    <row r="899" ht="14.25" customHeight="1"/>
+    <row r="900" ht="14.25" customHeight="1"/>
+    <row r="901" ht="14.25" customHeight="1"/>
+    <row r="902" ht="14.25" customHeight="1"/>
+    <row r="903" ht="14.25" customHeight="1"/>
+    <row r="904" ht="14.25" customHeight="1"/>
+    <row r="905" ht="14.25" customHeight="1"/>
+    <row r="906" ht="14.25" customHeight="1"/>
+    <row r="907" ht="14.25" customHeight="1"/>
+    <row r="908" ht="14.25" customHeight="1"/>
+    <row r="909" ht="14.25" customHeight="1"/>
+    <row r="910" ht="14.25" customHeight="1"/>
+    <row r="911" ht="14.25" customHeight="1"/>
+    <row r="912" ht="14.25" customHeight="1"/>
+    <row r="913" ht="14.25" customHeight="1"/>
+    <row r="914" ht="14.25" customHeight="1"/>
+    <row r="915" ht="14.25" customHeight="1"/>
+    <row r="916" ht="14.25" customHeight="1"/>
+    <row r="917" ht="14.25" customHeight="1"/>
+    <row r="918" ht="14.25" customHeight="1"/>
+    <row r="919" ht="14.25" customHeight="1"/>
+    <row r="920" ht="14.25" customHeight="1"/>
+    <row r="921" ht="14.25" customHeight="1"/>
+    <row r="922" ht="14.25" customHeight="1"/>
+    <row r="923" ht="14.25" customHeight="1"/>
+    <row r="924" ht="14.25" customHeight="1"/>
+    <row r="925" ht="14.25" customHeight="1"/>
+    <row r="926" ht="14.25" customHeight="1"/>
+    <row r="927" ht="14.25" customHeight="1"/>
+    <row r="928" ht="14.25" customHeight="1"/>
+    <row r="929" ht="14.25" customHeight="1"/>
+    <row r="930" ht="14.25" customHeight="1"/>
+    <row r="931" ht="14.25" customHeight="1"/>
+    <row r="932" ht="14.25" customHeight="1"/>
+    <row r="933" ht="14.25" customHeight="1"/>
+    <row r="934" ht="14.25" customHeight="1"/>
+    <row r="935" ht="14.25" customHeight="1"/>
+    <row r="936" ht="14.25" customHeight="1"/>
+    <row r="937" ht="14.25" customHeight="1"/>
+    <row r="938" ht="14.25" customHeight="1"/>
+    <row r="939" ht="14.25" customHeight="1"/>
+    <row r="940" ht="14.25" customHeight="1"/>
+    <row r="941" ht="14.25" customHeight="1"/>
+    <row r="942" ht="14.25" customHeight="1"/>
+    <row r="943" ht="14.25" customHeight="1"/>
+    <row r="944" ht="14.25" customHeight="1"/>
+    <row r="945" ht="14.25" customHeight="1"/>
+    <row r="946" ht="14.25" customHeight="1"/>
+    <row r="947" ht="14.25" customHeight="1"/>
+    <row r="948" ht="14.25" customHeight="1"/>
+    <row r="949" ht="14.25" customHeight="1"/>
+    <row r="950" ht="14.25" customHeight="1"/>
+    <row r="951" ht="14.25" customHeight="1"/>
+    <row r="952" ht="14.25" customHeight="1"/>
+    <row r="953" ht="14.25" customHeight="1"/>
+    <row r="954" ht="14.25" customHeight="1"/>
+    <row r="955" ht="14.25" customHeight="1"/>
+    <row r="956" ht="14.25" customHeight="1"/>
+    <row r="957" ht="14.25" customHeight="1"/>
+    <row r="958" ht="14.25" customHeight="1"/>
+    <row r="959" ht="14.25" customHeight="1"/>
+    <row r="960" ht="14.25" customHeight="1"/>
+    <row r="961" ht="14.25" customHeight="1"/>
+    <row r="962" ht="14.25" customHeight="1"/>
+    <row r="963" ht="14.25" customHeight="1"/>
+    <row r="964" ht="14.25" customHeight="1"/>
+    <row r="965" ht="14.25" customHeight="1"/>
+    <row r="966" ht="14.25" customHeight="1"/>
+    <row r="967" ht="14.25" customHeight="1"/>
+    <row r="968" ht="14.25" customHeight="1"/>
+    <row r="969" ht="14.25" customHeight="1"/>
+    <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
+    <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
+    <row r="974" ht="14.25" customHeight="1"/>
+    <row r="975" ht="14.25" customHeight="1"/>
+    <row r="976" ht="14.25" customHeight="1"/>
+    <row r="977" ht="14.25" customHeight="1"/>
+    <row r="978" ht="14.25" customHeight="1"/>
+    <row r="979" ht="14.25" customHeight="1"/>
+    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="981" ht="14.25" customHeight="1"/>
+    <row r="982" ht="14.25" customHeight="1"/>
+    <row r="983" ht="14.25" customHeight="1"/>
+    <row r="984" ht="14.25" customHeight="1"/>
+    <row r="985" ht="14.25" customHeight="1"/>
+    <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed polarity of J5, changed values of R4 and R5 to 3k9, R19 and R20 to NF, changed part number of the GPS module to GT-1110-UB7X.
</commit_message>
<xml_diff>
--- a/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
+++ b/Hardware/Released Files/Assembly_Variant_Default/BOM/X2E Reference Sensor_Default_Bill of Materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\Altium\x2e-reference-sensor\Hardware\Released Files\Assembly_Variant_Default\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B19C6071-7C4C-4E81-8B57-43CA55A07E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B607C384-4BBA-4938-BAE1-89DB7AD06696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1885" yWindow="1885" windowWidth="21378" windowHeight="11387"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="338">
   <si>
     <t>Fitted</t>
   </si>
@@ -789,7 +789,28 @@
     <t>RE0402FRE0710KL</t>
   </si>
   <si>
-    <t>R4, R5, R7, R23</t>
+    <t>R4, R5</t>
+  </si>
+  <si>
+    <t>3k9</t>
+  </si>
+  <si>
+    <t>RES, 3k9, 1%, 0.063 W, 0603</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>3k</t>
+  </si>
+  <si>
+    <t>RES, 3k, 1%, 0.063 W, 0603</t>
+  </si>
+  <si>
+    <t>AF0603FR-073KL</t>
+  </si>
+  <si>
+    <t>R7, R23</t>
   </si>
   <si>
     <t>2k</t>
@@ -801,18 +822,6 @@
     <t>RE0603FRE072KL</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>3k</t>
-  </si>
-  <si>
-    <t>RES, 3k, 1%, 0.063 W, 0603</t>
-  </si>
-  <si>
-    <t>AF0603FR-073KL</t>
-  </si>
-  <si>
     <t>R8, R12, R15, R21, R30, R31, R39, R40, R49, R50, R69, R75, R83, R84</t>
   </si>
   <si>
@@ -861,7 +870,16 @@
     <t>AC0402FR-13100KL</t>
   </si>
   <si>
-    <t>R19, R20, R27, R28</t>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>RES, 1k, 1%, 1/16 W, 0402</t>
+  </si>
+  <si>
+    <t>R27, R28</t>
   </si>
   <si>
     <t>5k1</t>
@@ -873,15 +891,6 @@
     <t>AC0603FR-135K1L</t>
   </si>
   <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>RES, 1k, 1%, 1/16 W, 0402</t>
-  </si>
-  <si>
     <t>R33, R34, R37, R38, R43, R44, R72, R73, R74, R76, R77, R78</t>
   </si>
   <si>
@@ -972,13 +981,16 @@
     <t>U2</t>
   </si>
   <si>
+    <t>GT-1110-UB7X</t>
+  </si>
+  <si>
+    <t>GPS, GLONASS, QZSS and SBAS Module</t>
+  </si>
+  <si>
     <t>SIM28ML</t>
   </si>
   <si>
-    <t>GPS Module 10.1x9.7x2.5mm 9600 Baud Rate</t>
-  </si>
-  <si>
-    <t>SIMCom</t>
+    <t>GOTOP</t>
   </si>
   <si>
     <t>Y1</t>
@@ -1407,7 +1419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2729,7 +2741,7 @@
         <v>253</v>
       </c>
       <c r="C56" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>254</v>
@@ -2742,152 +2754,152 @@
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="2" t="s">
-        <v>256</v>
+        <v>24</v>
       </c>
       <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C57" s="1">
-        <v>1</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>246</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C58" s="1">
-        <v>14</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="F58" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" s="1">
+        <v>14</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C59" s="1">
-        <v>5</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>251</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I59" s="1"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C60" s="1">
+        <v>5</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C60" s="1">
-        <v>4</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>251</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I60" s="1"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C61" s="1">
+        <v>4</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C61" s="1">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>251</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I61" s="1"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C62" s="1">
-        <v>4</v>
-      </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="F62" s="2" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C63" s="1">
         <v>1</v>
@@ -2908,7 +2920,7 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
@@ -2917,7 +2929,7 @@
         <v>244</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>251</v>
@@ -2929,140 +2941,138 @@
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C65" s="1">
+        <v>2</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C65" s="1">
-        <v>12</v>
-      </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>286</v>
-      </c>
       <c r="F65" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C66" s="1">
+        <v>12</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C66" s="1">
-        <v>1</v>
-      </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>251</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C67" s="1">
-        <v>1</v>
-      </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>294</v>
-      </c>
       <c r="F67" s="2" t="s">
-        <v>295</v>
+        <v>251</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I67" s="1"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C69" s="1">
-        <v>2</v>
-      </c>
-      <c r="D69" s="1"/>
       <c r="E69" s="2" t="s">
         <v>302</v>
       </c>
       <c r="F69" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G69" s="1"/>
+      <c r="H69" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="I69" s="1"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C70" s="1">
         <v>2</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="D70" s="1"/>
       <c r="E70" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="I70" s="1"/>
     </row>
@@ -3072,9 +3082,11 @@
         <v>309</v>
       </c>
       <c r="C71" s="1">
-        <v>1</v>
-      </c>
-      <c r="D71" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E71" s="2" t="s">
         <v>310</v>
       </c>
@@ -3082,32 +3094,30 @@
         <v>311</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>312</v>
+        <v>24</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>311</v>
+        <v>24</v>
       </c>
       <c r="I71" s="1"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="C72" s="1">
-        <v>1</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>314</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>314</v>
@@ -3117,77 +3127,102 @@
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C73" s="1">
-        <v>1</v>
-      </c>
-      <c r="D73" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="G73" s="2" t="s">
-        <v>321</v>
-      </c>
       <c r="H73" s="2" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="I73" s="1"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C74" s="1">
-        <v>1</v>
-      </c>
-      <c r="D74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>328</v>
       </c>
       <c r="I74" s="1"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C75" s="1">
-        <v>1</v>
-      </c>
-      <c r="D75" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="G75" s="2" t="s">
+      <c r="H75" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="I75" s="1"/>
+      <c r="C76" s="1">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="I76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>